<commit_message>
updated time tables && add event type
</commit_message>
<xml_diff>
--- a/raw/time_tables/B.Tech (btech)/2/1.xlsx
+++ b/raw/time_tables/B.Tech (btech)/2/1.xlsx
@@ -2,10 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
-  <fileSharing readOnlyRecommended="1"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12420"/>
+    <workbookView windowWidth="14340" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Phase 1" sheetId="2" r:id="rId1"/>
@@ -16,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="577">
   <si>
     <t>B.TECH II SEMESTER EVEN 2025</t>
   </si>
@@ -135,7 +134,7 @@
     <t>LB5,B6(MA211)- FF4/RSC</t>
   </si>
   <si>
-    <t>LB3,B4(CI121)-FF2/AMT</t>
+    <t>LB3,B4(CI121)-LT2/AMT</t>
   </si>
   <si>
     <t>LA15,A16(PH211)-FF2/SDC</t>
@@ -168,7 +167,7 @@
     <t>TB6(B11HS111)-TS7/AMN</t>
   </si>
   <si>
-    <t>TB3(B11HS111)-TS6/IJ</t>
+    <t>TB3(B11HS111)-TS6/AMN</t>
   </si>
   <si>
     <t>TB7(B11HS111)-TS6/VSE</t>
@@ -426,9 +425,6 @@
     <t>TB11(CI121)-TS6/SHP</t>
   </si>
   <si>
-    <t>TA7(B11HS111)-TS12/PRI</t>
-  </si>
-  <si>
     <t>TA1(B11HS111)-TS8/AMN</t>
   </si>
   <si>
@@ -741,6 +737,9 @@
     <t>PA6 (HS111)- CL12/ PSH</t>
   </si>
   <si>
+    <t xml:space="preserve">LB5,B6(PH211)-G9/ABH </t>
+  </si>
+  <si>
     <t>PB3(CI271)-CL02/HN,TAJ,AA</t>
   </si>
   <si>
@@ -771,9 +770,6 @@
     <t>THU</t>
   </si>
   <si>
-    <t xml:space="preserve">LB5,B6(PH211)-G1/ABH </t>
-  </si>
-  <si>
     <t xml:space="preserve">LA17,A18(PH211)-G1/INC </t>
   </si>
   <si>
@@ -972,6 +968,9 @@
     <t>PB2(GE111)- CAD2/ GGL</t>
   </si>
   <si>
+    <t>LG1,G2(PH211)-G9/DIN</t>
+  </si>
+  <si>
     <t>PB7(GE111)- CAD1/ SWET</t>
   </si>
   <si>
@@ -1116,7 +1115,7 @@
     <t>PC1(CI121)- CL05/ALK,SON,PK</t>
   </si>
   <si>
-    <t>TC2(B11HS111)- TS13/AMN</t>
+    <t>TC2(B11HS111)- TS13/IJ</t>
   </si>
   <si>
     <t>PC2(B15BT111)- BT3/EKT, PMG,SHD,AKT</t>
@@ -1125,16 +1124,19 @@
     <t>TC3(B11HS111)- TS14/PRI</t>
   </si>
   <si>
+    <t>TA7(B11HS111)-TS16/PRI</t>
+  </si>
+  <si>
     <t>PG1(CI271)-CL05/GZL,DEP,AMS</t>
   </si>
   <si>
-    <t>PB9(HS111)- / HK</t>
+    <t>PB9(HS111)- LL/ HK</t>
   </si>
   <si>
     <t>PG2(CI271)-CL06 /NSA,APR,PAG</t>
   </si>
   <si>
-    <t>PB10(HS111)- / EKS</t>
+    <t>PB10(HS111)- CL12/ EKS</t>
   </si>
   <si>
     <t>PA5(PH271)-PL1 /MKC/SDC</t>
@@ -1751,10 +1753,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1829,15 +1831,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <charset val="134"/>
     </font>
@@ -1871,18 +1873,17 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1891,14 +1892,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1911,9 +1904,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1925,29 +1926,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1963,9 +1942,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1973,21 +1952,6 @@
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1999,12 +1963,66 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <charset val="1"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -2017,22 +2035,6 @@
       <color indexed="23"/>
       <name val="Calibri"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="39">
@@ -2080,19 +2082,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2104,7 +2106,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2122,6 +2124,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2134,7 +2142,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2146,19 +2160,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2170,49 +2214,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2224,13 +2244,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2242,25 +2256,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2944,15 +2946,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2987,11 +2980,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3010,23 +3009,26 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3037,154 +3039,154 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="58" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="58" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="57" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="56" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="16" borderId="59" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="55" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="55" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="54" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="54" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="53" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="54" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="17" borderId="53" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="56" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="59" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="57" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="57" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="52" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="52" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="240">
+  <cellXfs count="244">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3384,6 +3386,9 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3612,6 +3617,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -3678,7 +3692,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3781,13 +3795,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3808,13 +3822,13 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3860,6 +3874,10 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3872,13 +3890,13 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3887,10 +3905,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="53">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4251,11 +4265,11 @@
   <dimension ref="A1:L191"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B127" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C120" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K153" sqref="K153"/>
+      <selection pane="bottomRight" activeCell="F154" sqref="F154:F161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="14.25"/>
@@ -4286,7 +4300,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="107"/>
+      <c r="I1" s="108"/>
     </row>
     <row r="2" ht="15" spans="1:9">
       <c r="A2" s="5"/>
@@ -4299,10 +4313,10 @@
       <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="70" t="s">
+      <c r="E2" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="71" t="s">
+      <c r="F2" s="72" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="7" t="s">
@@ -4311,7 +4325,7 @@
       <c r="H2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="108" t="s">
+      <c r="I2" s="109" t="s">
         <v>8</v>
       </c>
     </row>
@@ -4328,7 +4342,7 @@
       <c r="D3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="72" t="s">
+      <c r="E3" s="73" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="10" t="s">
@@ -4340,7 +4354,7 @@
       <c r="H3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="109" t="s">
+      <c r="I3" s="110" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4355,7 +4369,7 @@
       <c r="D4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="73"/>
+      <c r="E4" s="74"/>
       <c r="F4" s="14" t="s">
         <v>21</v>
       </c>
@@ -4365,7 +4379,7 @@
       <c r="H4" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="110" t="s">
+      <c r="I4" s="111" t="s">
         <v>24</v>
       </c>
     </row>
@@ -4380,7 +4394,7 @@
       <c r="D5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="73"/>
+      <c r="E5" s="74"/>
       <c r="F5" s="18" t="s">
         <v>28</v>
       </c>
@@ -4390,7 +4404,7 @@
       <c r="H5" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="111"/>
+      <c r="I5" s="112"/>
     </row>
     <row r="6" ht="33.75" customHeight="1" spans="1:9">
       <c r="A6" s="11"/>
@@ -4403,7 +4417,7 @@
       <c r="D6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="73"/>
+      <c r="E6" s="74"/>
       <c r="F6" s="14" t="s">
         <v>34</v>
       </c>
@@ -4413,7 +4427,7 @@
       <c r="H6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="112" t="s">
+      <c r="I6" s="113" t="s">
         <v>37</v>
       </c>
     </row>
@@ -4428,13 +4442,13 @@
       <c r="D7" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="73"/>
+      <c r="E7" s="74"/>
       <c r="F7" s="14" t="s">
         <v>41</v>
       </c>
       <c r="G7" s="18"/>
       <c r="H7" s="14"/>
-      <c r="I7" s="112" t="s">
+      <c r="I7" s="113" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4447,15 +4461,15 @@
       <c r="D8" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="73"/>
-      <c r="F8" s="74" t="s">
+      <c r="E8" s="74"/>
+      <c r="F8" s="75" t="s">
         <v>45</v>
       </c>
       <c r="G8" s="18"/>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="76" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="112" t="s">
+      <c r="I8" s="113" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4467,17 +4481,17 @@
       <c r="C9" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="73"/>
+      <c r="E9" s="74"/>
       <c r="F9" s="18" t="s">
         <v>50</v>
       </c>
       <c r="G9" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="75" t="s">
+      <c r="H9" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="112" t="s">
+      <c r="I9" s="113" t="s">
         <v>53</v>
       </c>
     </row>
@@ -4492,15 +4506,15 @@
       <c r="D10" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="73"/>
+      <c r="E10" s="74"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="75" t="s">
+      <c r="G10" s="76" t="s">
         <v>57</v>
       </c>
       <c r="H10" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="111" t="s">
+      <c r="I10" s="112" t="s">
         <v>59</v>
       </c>
     </row>
@@ -4513,13 +4527,13 @@
       <c r="D11" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="E11" s="73"/>
+      <c r="E11" s="74"/>
       <c r="F11" s="18"/>
       <c r="G11" s="18"/>
       <c r="H11" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="I11" s="111"/>
+      <c r="I11" s="112"/>
     </row>
     <row r="12" ht="33.75" customHeight="1" spans="1:9">
       <c r="A12" s="11"/>
@@ -4530,13 +4544,13 @@
       <c r="D12" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="E12" s="73"/>
+      <c r="E12" s="74"/>
       <c r="F12" s="18"/>
-      <c r="G12" s="76" t="s">
+      <c r="G12" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="H12" s="76"/>
-      <c r="I12" s="111"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="112"/>
     </row>
     <row r="13" ht="33.75" customHeight="1" spans="1:9">
       <c r="A13" s="11"/>
@@ -4547,13 +4561,13 @@
       <c r="D13" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="73"/>
+      <c r="E13" s="74"/>
       <c r="F13" s="18"/>
-      <c r="G13" s="76" t="s">
+      <c r="G13" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="H13" s="76"/>
-      <c r="I13" s="111"/>
+      <c r="H13" s="77"/>
+      <c r="I13" s="112"/>
     </row>
     <row r="14" ht="36" customHeight="1" spans="1:9">
       <c r="A14" s="11"/>
@@ -4564,13 +4578,13 @@
       <c r="D14" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="73"/>
+      <c r="E14" s="74"/>
       <c r="F14" s="46"/>
-      <c r="G14" s="77" t="s">
+      <c r="G14" s="78" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="77"/>
-      <c r="I14" s="111"/>
+      <c r="H14" s="78"/>
+      <c r="I14" s="112"/>
     </row>
     <row r="15" ht="32.25" customHeight="1" spans="1:9">
       <c r="A15" s="11"/>
@@ -4579,7 +4593,7 @@
         <v>72</v>
       </c>
       <c r="D15" s="30"/>
-      <c r="E15" s="73"/>
+      <c r="E15" s="74"/>
       <c r="F15" s="18" t="s">
         <v>73</v>
       </c>
@@ -4587,7 +4601,7 @@
       <c r="H15" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="I15" s="113"/>
+      <c r="I15" s="114"/>
     </row>
     <row r="16" ht="19.5" customHeight="1" spans="1:9">
       <c r="A16" s="11"/>
@@ -4596,7 +4610,7 @@
         <v>75</v>
       </c>
       <c r="D16" s="30"/>
-      <c r="E16" s="73"/>
+      <c r="E16" s="74"/>
       <c r="F16" s="18" t="s">
         <v>76</v>
       </c>
@@ -4604,7 +4618,7 @@
       <c r="H16" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="I16" s="113"/>
+      <c r="I16" s="114"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="11"/>
@@ -4613,7 +4627,7 @@
       </c>
       <c r="C17" s="31"/>
       <c r="D17" s="29"/>
-      <c r="E17" s="73"/>
+      <c r="E17" s="74"/>
       <c r="F17" s="14" t="s">
         <v>79</v>
       </c>
@@ -4621,7 +4635,7 @@
       <c r="H17" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="I17" s="113"/>
+      <c r="I17" s="114"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="11"/>
@@ -4630,7 +4644,7 @@
       </c>
       <c r="C18" s="31"/>
       <c r="D18" s="18"/>
-      <c r="E18" s="73"/>
+      <c r="E18" s="74"/>
       <c r="F18" s="14" t="s">
         <v>82</v>
       </c>
@@ -4638,20 +4652,20 @@
       <c r="H18" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="I18" s="113"/>
+      <c r="I18" s="114"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="11"/>
       <c r="B19" s="17"/>
       <c r="C19" s="18"/>
       <c r="D19" s="18"/>
-      <c r="E19" s="73"/>
+      <c r="E19" s="74"/>
       <c r="F19" s="29"/>
       <c r="G19" s="29"/>
       <c r="H19" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="I19" s="114"/>
+      <c r="I19" s="115"/>
     </row>
     <row r="20" ht="29.25" customHeight="1" spans="1:9">
       <c r="A20" s="11"/>
@@ -4660,13 +4674,13 @@
       </c>
       <c r="C20" s="33"/>
       <c r="D20" s="34"/>
-      <c r="E20" s="73"/>
+      <c r="E20" s="74"/>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
       <c r="H20" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="I20" s="114"/>
+      <c r="I20" s="115"/>
     </row>
     <row r="21" ht="24" customHeight="1" spans="1:9">
       <c r="A21" s="35"/>
@@ -4675,13 +4689,13 @@
       </c>
       <c r="C21" s="36"/>
       <c r="D21" s="36"/>
-      <c r="E21" s="73"/>
+      <c r="E21" s="74"/>
       <c r="F21" s="32" t="s">
         <v>88</v>
       </c>
       <c r="G21" s="33"/>
       <c r="H21" s="34"/>
-      <c r="I21" s="115"/>
+      <c r="I21" s="116"/>
     </row>
     <row r="22" ht="24" customHeight="1" spans="1:9">
       <c r="A22" s="37"/>
@@ -4690,34 +4704,34 @@
       </c>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
-      <c r="E22" s="73"/>
+      <c r="E22" s="74"/>
       <c r="F22" s="36" t="s">
         <v>90</v>
       </c>
       <c r="G22" s="36"/>
       <c r="H22" s="36"/>
-      <c r="I22" s="115"/>
+      <c r="I22" s="116"/>
     </row>
     <row r="23" ht="22.5" customHeight="1" spans="1:9">
       <c r="A23" s="39"/>
-      <c r="E23" s="73"/>
+      <c r="E23" s="74"/>
       <c r="F23" s="48" t="s">
         <v>91</v>
       </c>
       <c r="G23" s="49"/>
       <c r="H23" s="50"/>
-      <c r="I23" s="116"/>
+      <c r="I23" s="117"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="8.25" customHeight="1" spans="1:9">
       <c r="A24" s="40"/>
       <c r="B24" s="41"/>
       <c r="C24" s="42"/>
       <c r="D24" s="42"/>
-      <c r="E24" s="78"/>
+      <c r="E24" s="79"/>
       <c r="F24" s="42"/>
       <c r="G24" s="42"/>
       <c r="H24" s="42"/>
-      <c r="I24" s="117"/>
+      <c r="I24" s="118"/>
     </row>
     <row r="25" ht="34.5" customHeight="1" spans="1:9">
       <c r="A25" s="8" t="s">
@@ -4732,7 +4746,7 @@
       <c r="D25" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="79" t="s">
+      <c r="E25" s="80" t="s">
         <v>13</v>
       </c>
       <c r="F25" s="14" t="s">
@@ -4744,7 +4758,7 @@
       <c r="H25" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="I25" s="110" t="s">
+      <c r="I25" s="111" t="s">
         <v>98</v>
       </c>
     </row>
@@ -4759,7 +4773,7 @@
       <c r="D26" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="E26" s="73"/>
+      <c r="E26" s="74"/>
       <c r="F26" s="14" t="s">
         <v>102</v>
       </c>
@@ -4769,7 +4783,7 @@
       <c r="H26" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="I26" s="110" t="s">
+      <c r="I26" s="111" t="s">
         <v>32</v>
       </c>
     </row>
@@ -4784,7 +4798,7 @@
       <c r="D27" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="E27" s="73"/>
+      <c r="E27" s="74"/>
       <c r="F27" s="14" t="s">
         <v>108</v>
       </c>
@@ -4794,7 +4808,7 @@
       <c r="H27" s="18" t="s">
         <v>110</v>
       </c>
-      <c r="I27" s="110" t="s">
+      <c r="I27" s="111" t="s">
         <v>111</v>
       </c>
     </row>
@@ -4809,7 +4823,7 @@
       <c r="D28" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="73"/>
+      <c r="E28" s="74"/>
       <c r="F28" s="14" t="s">
         <v>115</v>
       </c>
@@ -4832,15 +4846,15 @@
       <c r="D29" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="E29" s="73"/>
-      <c r="F29" s="80"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="81"/>
       <c r="G29" s="14" t="s">
         <v>121</v>
       </c>
       <c r="H29" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="I29" s="112" t="s">
+      <c r="I29" s="113" t="s">
         <v>123</v>
       </c>
     </row>
@@ -4855,8 +4869,8 @@
       <c r="D30" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="E30" s="73"/>
-      <c r="F30" s="81" t="s">
+      <c r="E30" s="74"/>
+      <c r="F30" s="82" t="s">
         <v>127</v>
       </c>
       <c r="G30" s="14" t="s">
@@ -4865,7 +4879,7 @@
       <c r="H30" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="I30" s="111" t="s">
+      <c r="I30" s="112" t="s">
         <v>130</v>
       </c>
     </row>
@@ -4880,465 +4894,463 @@
       <c r="D31" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="E31" s="73"/>
-      <c r="F31" s="75" t="s">
+      <c r="E31" s="74"/>
+      <c r="F31" s="76" t="s">
         <v>134</v>
       </c>
       <c r="G31" s="18"/>
-      <c r="H31" s="82" t="s">
+      <c r="H31" s="83" t="s">
         <v>135</v>
       </c>
-      <c r="I31" s="118" t="s">
-        <v>136</v>
-      </c>
+      <c r="I31" s="119"/>
     </row>
     <row r="32" ht="39.75" customHeight="1" spans="1:9">
       <c r="A32" s="11"/>
       <c r="B32" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="D32" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="D32" s="46" t="s">
+      <c r="E32" s="74"/>
+      <c r="F32" s="84" t="s">
         <v>139</v>
       </c>
-      <c r="E32" s="73"/>
-      <c r="F32" s="83" t="s">
+      <c r="G32" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="G32" s="18" t="s">
+      <c r="H32" s="85"/>
+      <c r="I32" s="119" t="s">
         <v>141</v>
-      </c>
-      <c r="H32" s="84"/>
-      <c r="I32" s="118" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="33" ht="39.75" customHeight="1" spans="1:9">
       <c r="A33" s="11"/>
       <c r="B33" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C33" s="18" t="s">
         <v>143</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="D33" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="D33" s="46" t="s">
-        <v>145</v>
-      </c>
-      <c r="E33" s="73"/>
+      <c r="E33" s="74"/>
       <c r="F33" s="18"/>
       <c r="G33" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="H33" s="76" t="s">
         <v>146</v>
       </c>
-      <c r="H33" s="75" t="s">
+      <c r="I33" s="113" t="s">
         <v>147</v>
-      </c>
-      <c r="I33" s="112" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="34" ht="25.5" customHeight="1" spans="1:9">
       <c r="A34" s="11"/>
       <c r="B34" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="C34" s="30" t="s">
+      <c r="D34" s="30"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="87" t="s">
         <v>150</v>
       </c>
-      <c r="D34" s="30"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="86" t="s">
+      <c r="H34" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="H34" s="75" t="s">
-        <v>152</v>
-      </c>
-      <c r="I34" s="111"/>
+      <c r="I34" s="112"/>
     </row>
     <row r="35" ht="33" customHeight="1" spans="1:9">
       <c r="A35" s="11"/>
       <c r="B35" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C35" s="31"/>
       <c r="D35" s="13"/>
-      <c r="E35" s="73"/>
+      <c r="E35" s="74"/>
       <c r="F35" s="18"/>
-      <c r="G35" s="75" t="s">
+      <c r="G35" s="76" t="s">
+        <v>153</v>
+      </c>
+      <c r="H35" s="88" t="s">
         <v>154</v>
       </c>
-      <c r="H35" s="87" t="s">
-        <v>155</v>
-      </c>
-      <c r="I35" s="119"/>
+      <c r="I35" s="120"/>
     </row>
     <row r="36" ht="29.25" customHeight="1" spans="1:9">
       <c r="A36" s="11"/>
       <c r="B36" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C36" s="31"/>
       <c r="D36" s="18"/>
-      <c r="E36" s="73"/>
+      <c r="E36" s="74"/>
       <c r="F36" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="G36" s="31"/>
+      <c r="H36" s="89" t="s">
         <v>157</v>
       </c>
-      <c r="G36" s="31"/>
-      <c r="H36" s="88" t="s">
-        <v>158</v>
-      </c>
-      <c r="I36" s="120"/>
+      <c r="I36" s="121"/>
     </row>
     <row r="37" customHeight="1" spans="1:9">
       <c r="A37" s="11"/>
       <c r="B37" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C37" s="31"/>
       <c r="D37" s="18"/>
-      <c r="E37" s="73"/>
+      <c r="E37" s="74"/>
       <c r="F37" s="31" t="s">
+        <v>159</v>
+      </c>
+      <c r="G37" s="31"/>
+      <c r="H37" s="90" t="s">
         <v>160</v>
       </c>
-      <c r="G37" s="31"/>
-      <c r="H37" s="89" t="s">
-        <v>161</v>
-      </c>
-      <c r="I37" s="121"/>
+      <c r="I37" s="122"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="11"/>
       <c r="B38" s="27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C38" s="31"/>
       <c r="D38" s="18"/>
-      <c r="E38" s="73"/>
+      <c r="E38" s="74"/>
       <c r="F38" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="G38" s="30"/>
+      <c r="H38" s="91" t="s">
         <v>163</v>
       </c>
-      <c r="G38" s="30"/>
-      <c r="H38" s="90" t="s">
-        <v>164</v>
-      </c>
-      <c r="I38" s="122"/>
+      <c r="I38" s="123"/>
     </row>
     <row r="39" ht="21.75" customHeight="1" spans="1:9">
       <c r="A39" s="11"/>
       <c r="B39" s="47"/>
       <c r="C39" s="30" t="s">
+        <v>164</v>
+      </c>
+      <c r="D39" s="30"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="73"/>
-      <c r="F39" s="30" t="s">
+      <c r="G39" s="30"/>
+      <c r="H39" s="89" t="s">
         <v>166</v>
       </c>
-      <c r="G39" s="30"/>
-      <c r="H39" s="88" t="s">
-        <v>167</v>
-      </c>
-      <c r="I39" s="120"/>
+      <c r="I39" s="121"/>
     </row>
     <row r="40" ht="28.5" customHeight="1" spans="1:9">
       <c r="A40" s="11"/>
       <c r="B40" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C40" s="33"/>
       <c r="D40" s="34"/>
-      <c r="E40" s="73"/>
+      <c r="E40" s="74"/>
       <c r="F40" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G40" s="33"/>
       <c r="H40" s="34"/>
-      <c r="I40" s="123"/>
+      <c r="I40" s="124"/>
     </row>
     <row r="41" ht="30" customHeight="1" spans="1:9">
       <c r="A41" s="11"/>
       <c r="B41" s="36" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C41" s="36"/>
       <c r="D41" s="36"/>
-      <c r="E41" s="73"/>
+      <c r="E41" s="74"/>
       <c r="F41" s="36" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G41" s="36"/>
       <c r="H41" s="36"/>
-      <c r="I41" s="116"/>
+      <c r="I41" s="117"/>
     </row>
     <row r="42" ht="26.25" customHeight="1" spans="1:9">
       <c r="A42" s="39"/>
       <c r="B42" s="48" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C42" s="49"/>
       <c r="D42" s="50"/>
-      <c r="E42" s="91"/>
+      <c r="E42" s="92"/>
       <c r="F42" s="48" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G42" s="49"/>
       <c r="H42" s="50"/>
-      <c r="I42" s="115"/>
+      <c r="I42" s="116"/>
     </row>
     <row r="43" s="1" customFormat="1" ht="7.5" customHeight="1" spans="1:9">
       <c r="A43" s="51"/>
       <c r="B43" s="52"/>
       <c r="C43" s="53"/>
       <c r="D43" s="53"/>
-      <c r="E43" s="92"/>
-      <c r="F43" s="93"/>
-      <c r="G43" s="93"/>
-      <c r="H43" s="93"/>
-      <c r="I43" s="124"/>
+      <c r="E43" s="93"/>
+      <c r="F43" s="94"/>
+      <c r="G43" s="94"/>
+      <c r="H43" s="94"/>
+      <c r="I43" s="125"/>
     </row>
     <row r="44" ht="26.25" customHeight="1" spans="1:9">
       <c r="A44" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="B44" s="54" t="s">
         <v>174</v>
-      </c>
-      <c r="B44" s="54" t="s">
-        <v>175</v>
       </c>
       <c r="C44" s="55" t="s">
         <v>96</v>
       </c>
       <c r="D44" s="55" t="s">
+        <v>175</v>
+      </c>
+      <c r="E44" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="96" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="E44" s="94" t="s">
-        <v>13</v>
-      </c>
-      <c r="F44" s="95" t="s">
-        <v>14</v>
-      </c>
-      <c r="G44" s="55" t="s">
+      <c r="H44" s="55" t="s">
         <v>177</v>
       </c>
-      <c r="H44" s="55" t="s">
+      <c r="I44" s="126" t="s">
         <v>178</v>
-      </c>
-      <c r="I44" s="125" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="45" ht="33" customHeight="1" spans="1:8">
       <c r="A45" s="11"/>
       <c r="B45" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="C45" s="55" t="s">
         <v>180</v>
       </c>
-      <c r="C45" s="55" t="s">
+      <c r="D45" s="56" t="s">
         <v>181</v>
       </c>
-      <c r="D45" s="56" t="s">
+      <c r="E45" s="95"/>
+      <c r="F45" s="14" t="s">
         <v>182</v>
       </c>
-      <c r="E45" s="94"/>
-      <c r="F45" s="14" t="s">
+      <c r="G45" s="97"/>
+      <c r="H45" s="55" t="s">
         <v>183</v>
-      </c>
-      <c r="G45" s="96"/>
-      <c r="H45" s="55" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="46" ht="32.25" customHeight="1" spans="1:9">
       <c r="A46" s="11"/>
       <c r="B46" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C46" s="14" t="s">
         <v>185</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="D46" s="55" t="s">
         <v>186</v>
       </c>
-      <c r="D46" s="55" t="s">
+      <c r="E46" s="95"/>
+      <c r="F46" s="98" t="s">
         <v>187</v>
       </c>
-      <c r="E46" s="94"/>
-      <c r="F46" s="97" t="s">
+      <c r="G46" s="14" t="s">
         <v>188</v>
       </c>
-      <c r="G46" s="14" t="s">
+      <c r="H46" s="55" t="s">
         <v>189</v>
       </c>
-      <c r="H46" s="55" t="s">
+      <c r="I46" s="127" t="s">
         <v>190</v>
-      </c>
-      <c r="I46" s="126" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="47" ht="39" customHeight="1" spans="1:9">
       <c r="A47" s="11"/>
       <c r="B47" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="C47" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="C47" s="18" t="s">
+      <c r="D47" s="14" t="s">
         <v>193</v>
       </c>
-      <c r="D47" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="E47" s="94"/>
+      <c r="E47" s="95"/>
       <c r="F47" s="63" t="s">
         <v>117</v>
       </c>
       <c r="G47" s="55" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H47" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="I47" s="110" t="s">
-        <v>196</v>
+      <c r="I47" s="111" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="48" ht="30" customHeight="1" spans="1:9">
       <c r="A48" s="11"/>
       <c r="B48" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C48" s="14" t="s">
         <v>197</v>
       </c>
-      <c r="C48" s="14" t="s">
+      <c r="D48" s="14" t="s">
         <v>198</v>
       </c>
-      <c r="D48" s="14" t="s">
+      <c r="E48" s="95"/>
+      <c r="F48" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="E48" s="94"/>
-      <c r="F48" s="14" t="s">
+      <c r="G48" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="G48" s="46" t="s">
+      <c r="H48" s="58" t="s">
         <v>201</v>
       </c>
-      <c r="H48" s="58" t="s">
+      <c r="I48" s="111" t="s">
         <v>202</v>
-      </c>
-      <c r="I48" s="110" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="49" ht="29.25" customHeight="1" spans="1:9">
       <c r="A49" s="11"/>
       <c r="B49" s="57" t="s">
+        <v>203</v>
+      </c>
+      <c r="C49" s="58" t="s">
         <v>204</v>
-      </c>
-      <c r="C49" s="58" t="s">
-        <v>205</v>
       </c>
       <c r="D49" s="59" t="s">
         <v>126</v>
       </c>
-      <c r="E49" s="94"/>
+      <c r="E49" s="95"/>
       <c r="F49" s="58" t="s">
+        <v>205</v>
+      </c>
+      <c r="G49" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="G49" s="14" t="s">
+      <c r="H49" s="99" t="s">
         <v>207</v>
       </c>
-      <c r="H49" s="98" t="s">
-        <v>208</v>
-      </c>
-      <c r="I49" s="123"/>
+      <c r="I49" s="124"/>
     </row>
     <row r="50" ht="41.25" customHeight="1" spans="1:9">
       <c r="A50" s="11"/>
       <c r="B50" s="60" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C50" s="61"/>
       <c r="D50" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="E50" s="95"/>
+      <c r="F50" s="98" t="s">
         <v>210</v>
       </c>
-      <c r="E50" s="94"/>
-      <c r="F50" s="97" t="s">
+      <c r="G50" s="64" t="s">
         <v>211</v>
       </c>
-      <c r="G50" s="64" t="s">
+      <c r="H50" s="99" t="s">
         <v>212</v>
       </c>
-      <c r="H50" s="98" t="s">
-        <v>213</v>
-      </c>
-      <c r="I50" s="127"/>
+      <c r="I50" s="128"/>
     </row>
     <row r="51" ht="41.25" customHeight="1" spans="1:9">
       <c r="A51" s="35"/>
       <c r="B51" s="62"/>
       <c r="C51" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="D51" s="18" t="s">
         <v>214</v>
       </c>
-      <c r="D51" s="18" t="s">
+      <c r="E51" s="95"/>
+      <c r="F51" s="56" t="s">
         <v>215</v>
       </c>
-      <c r="E51" s="94"/>
-      <c r="F51" s="56" t="s">
+      <c r="G51" s="100" t="s">
         <v>216</v>
       </c>
-      <c r="G51" s="99" t="s">
-        <v>217</v>
-      </c>
       <c r="H51" s="62"/>
-      <c r="I51" s="127"/>
+      <c r="I51" s="128"/>
     </row>
     <row r="52" ht="41.25" customHeight="1" spans="1:9">
       <c r="A52" s="35"/>
       <c r="B52" s="62"/>
       <c r="C52" s="20" t="s">
+        <v>217</v>
+      </c>
+      <c r="D52" s="63" t="s">
         <v>218</v>
       </c>
-      <c r="D52" s="63" t="s">
-        <v>219</v>
-      </c>
-      <c r="E52" s="94"/>
+      <c r="E52" s="95"/>
       <c r="F52" s="62"/>
       <c r="G52" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="H52" s="101" t="s">
         <v>220</v>
       </c>
-      <c r="H52" s="100" t="s">
-        <v>221</v>
-      </c>
-      <c r="I52" s="100"/>
+      <c r="I52" s="101"/>
     </row>
     <row r="53" ht="27.75" customHeight="1" spans="1:9">
       <c r="A53" s="11"/>
       <c r="B53" s="27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C53" s="31"/>
       <c r="D53" s="64" t="s">
-        <v>223</v>
-      </c>
-      <c r="E53" s="94"/>
+        <v>222</v>
+      </c>
+      <c r="E53" s="95"/>
       <c r="F53" s="62"/>
       <c r="G53" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="H53" s="101" t="s">
         <v>224</v>
       </c>
-      <c r="H53" s="100" t="s">
-        <v>225</v>
-      </c>
-      <c r="I53" s="100"/>
+      <c r="I53" s="101"/>
     </row>
     <row r="54" ht="26.25" customHeight="1" spans="1:9">
       <c r="A54" s="11"/>
       <c r="B54" s="27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C54" s="31"/>
       <c r="D54" s="64" t="s">
+        <v>226</v>
+      </c>
+      <c r="E54" s="95"/>
+      <c r="F54" s="62" t="s">
         <v>227</v>
-      </c>
-      <c r="E54" s="94"/>
-      <c r="F54" s="62" t="s">
-        <v>228</v>
       </c>
       <c r="G54" s="62"/>
       <c r="H54" s="62" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I54" s="62"/>
     </row>
@@ -5346,16 +5358,16 @@
       <c r="A55" s="11"/>
       <c r="B55" s="17"/>
       <c r="C55" s="62" t="s">
+        <v>229</v>
+      </c>
+      <c r="D55" s="62"/>
+      <c r="E55" s="95"/>
+      <c r="F55" s="31" t="s">
         <v>230</v>
-      </c>
-      <c r="D55" s="62"/>
-      <c r="E55" s="94"/>
-      <c r="F55" s="31" t="s">
-        <v>231</v>
       </c>
       <c r="G55" s="31"/>
       <c r="H55" s="62" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I55" s="62"/>
     </row>
@@ -5363,68 +5375,70 @@
       <c r="A56" s="11"/>
       <c r="B56" s="65"/>
       <c r="C56" s="62" t="s">
+        <v>232</v>
+      </c>
+      <c r="D56" s="62"/>
+      <c r="E56" s="95"/>
+      <c r="F56" s="31" t="s">
         <v>233</v>
-      </c>
-      <c r="D56" s="62"/>
-      <c r="E56" s="94"/>
-      <c r="F56" s="31" t="s">
-        <v>234</v>
       </c>
       <c r="G56" s="31"/>
       <c r="H56" s="31" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I56" s="31"/>
-      <c r="L56" s="128"/>
+      <c r="L56" s="129"/>
     </row>
     <row r="57" ht="33.75" customHeight="1" spans="1:12">
       <c r="A57" s="11"/>
       <c r="B57" s="27" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C57" s="31"/>
       <c r="D57" s="66" t="s">
-        <v>237</v>
-      </c>
-      <c r="E57" s="94"/>
+        <v>236</v>
+      </c>
+      <c r="E57" s="95"/>
       <c r="F57" s="62"/>
       <c r="G57" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="H57" s="31" t="s">
         <v>238</v>
       </c>
-      <c r="H57" s="31" t="s">
-        <v>239</v>
-      </c>
       <c r="I57" s="31"/>
-      <c r="L57" s="128"/>
-    </row>
-    <row r="58" customHeight="1" spans="1:12">
+      <c r="L57" s="129"/>
+    </row>
+    <row r="58" ht="26.25" customHeight="1" spans="1:12">
       <c r="A58" s="11"/>
       <c r="B58" s="27" t="s">
+        <v>239</v>
+      </c>
+      <c r="C58" s="31"/>
+      <c r="D58" s="67" t="s">
         <v>240</v>
       </c>
-      <c r="C58" s="31"/>
-      <c r="D58" s="18"/>
-      <c r="E58" s="94"/>
+      <c r="E58" s="95"/>
       <c r="F58" s="62"/>
       <c r="G58" s="62"/>
-      <c r="H58" s="100" t="s">
+      <c r="H58" s="101" t="s">
         <v>241</v>
       </c>
-      <c r="I58" s="100"/>
-      <c r="L58" s="129"/>
+      <c r="I58" s="101"/>
+      <c r="L58" s="130"/>
     </row>
     <row r="59" ht="20.25" customHeight="1" spans="1:9">
       <c r="A59" s="11"/>
-      <c r="B59" s="67"/>
+      <c r="B59" s="68"/>
       <c r="C59" s="62"/>
       <c r="D59" s="62"/>
-      <c r="E59" s="94"/>
+      <c r="E59" s="95"/>
       <c r="F59" s="62"/>
       <c r="G59" s="62"/>
-      <c r="H59" s="100" t="s">
+      <c r="H59" s="101" t="s">
         <v>242</v>
       </c>
-      <c r="I59" s="100"/>
+      <c r="I59" s="101"/>
     </row>
     <row r="60" ht="17.25" customHeight="1" spans="1:9">
       <c r="A60" s="11"/>
@@ -5433,7 +5447,7 @@
       </c>
       <c r="C60" s="33"/>
       <c r="D60" s="34"/>
-      <c r="E60" s="94"/>
+      <c r="E60" s="95"/>
       <c r="F60" s="62"/>
       <c r="G60" s="62" t="s">
         <v>244</v>
@@ -5448,12 +5462,12 @@
       </c>
       <c r="C61" s="36"/>
       <c r="D61" s="36"/>
-      <c r="E61" s="94"/>
-      <c r="G61" s="101" t="s">
+      <c r="E61" s="95"/>
+      <c r="G61" s="102" t="s">
         <v>246</v>
       </c>
-      <c r="H61" s="102"/>
-      <c r="I61" s="130"/>
+      <c r="H61" s="103"/>
+      <c r="I61" s="131"/>
     </row>
     <row r="62" ht="22.5" customHeight="1" spans="1:9">
       <c r="A62" s="37"/>
@@ -5462,8 +5476,8 @@
       </c>
       <c r="C62" s="38"/>
       <c r="D62" s="38"/>
-      <c r="E62" s="94"/>
-      <c r="F62" s="103"/>
+      <c r="E62" s="95"/>
+      <c r="F62" s="104"/>
       <c r="G62" s="38" t="s">
         <v>248</v>
       </c>
@@ -5472,8 +5486,8 @@
     </row>
     <row r="63" ht="24.75" customHeight="1" spans="1:9">
       <c r="A63" s="39"/>
-      <c r="E63" s="94"/>
-      <c r="F63" s="104"/>
+      <c r="E63" s="95"/>
+      <c r="F63" s="105"/>
       <c r="G63" s="36" t="s">
         <v>249</v>
       </c>
@@ -5482,353 +5496,350 @@
     </row>
     <row r="64" ht="16.5" customHeight="1" spans="1:9">
       <c r="A64" s="40"/>
-      <c r="B64" s="68"/>
-      <c r="C64" s="69"/>
-      <c r="D64" s="69"/>
-      <c r="E64" s="105"/>
+      <c r="B64" s="69"/>
+      <c r="C64" s="70"/>
+      <c r="D64" s="70"/>
+      <c r="E64" s="106"/>
       <c r="F64" s="53"/>
-      <c r="G64" s="106"/>
+      <c r="G64" s="107"/>
       <c r="H64" s="53"/>
-      <c r="I64" s="131"/>
+      <c r="I64" s="132"/>
     </row>
     <row r="65" ht="42.75" customHeight="1" spans="1:10">
       <c r="A65" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="D65" s="82" t="s">
         <v>251</v>
       </c>
-      <c r="D65" s="81" t="s">
+      <c r="E65" s="162" t="s">
+        <v>13</v>
+      </c>
+      <c r="F65" s="82" t="s">
         <v>252</v>
       </c>
-      <c r="E65" s="158" t="s">
-        <v>13</v>
-      </c>
-      <c r="F65" s="81" t="s">
-        <v>253</v>
-      </c>
       <c r="G65" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H65" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="I65" s="110" t="s">
-        <v>254</v>
+      <c r="I65" s="111" t="s">
+        <v>253</v>
       </c>
       <c r="J65" s="1"/>
     </row>
     <row r="66" ht="38.25" customHeight="1" spans="1:10">
       <c r="A66" s="11"/>
       <c r="B66" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="C66" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="D66" s="82" t="s">
         <v>256</v>
       </c>
-      <c r="D66" s="81" t="s">
-        <v>257</v>
-      </c>
-      <c r="E66" s="159"/>
+      <c r="E66" s="163"/>
       <c r="F66" s="14" t="s">
         <v>21</v>
       </c>
       <c r="H66" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="I66" s="113" t="s">
         <v>258</v>
-      </c>
-      <c r="I66" s="112" t="s">
-        <v>259</v>
       </c>
       <c r="J66" s="1"/>
     </row>
     <row r="67" ht="33" customHeight="1" spans="1:10">
       <c r="A67" s="11"/>
       <c r="B67" s="12" t="s">
+        <v>259</v>
+      </c>
+      <c r="C67" s="86" t="s">
         <v>260</v>
-      </c>
-      <c r="C67" s="85" t="s">
-        <v>261</v>
       </c>
       <c r="D67" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E67" s="159"/>
+      <c r="E67" s="163"/>
       <c r="F67" s="14" t="s">
+        <v>261</v>
+      </c>
+      <c r="G67" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="G67" s="14" t="s">
+      <c r="H67" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="H67" s="13" t="s">
+      <c r="I67" s="113" t="s">
         <v>264</v>
-      </c>
-      <c r="I67" s="112" t="s">
-        <v>265</v>
       </c>
       <c r="J67" s="1"/>
     </row>
     <row r="68" ht="37.5" customHeight="1" spans="1:10">
       <c r="A68" s="11"/>
-      <c r="B68" s="132" t="s">
+      <c r="B68" s="133" t="s">
+        <v>265</v>
+      </c>
+      <c r="C68" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="C68" s="14" t="s">
+      <c r="D68" s="14" t="s">
         <v>267</v>
       </c>
-      <c r="D68" s="14" t="s">
+      <c r="E68" s="163"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="E68" s="159"/>
-      <c r="F68" s="14" t="s">
+      <c r="H68" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="G68" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="H68" s="14" t="s">
+      <c r="I68" s="178" t="s">
         <v>270</v>
-      </c>
-      <c r="I68" s="174" t="s">
-        <v>271</v>
       </c>
       <c r="J68" s="1"/>
     </row>
     <row r="69" ht="36.75" customHeight="1" spans="1:10">
       <c r="A69" s="11"/>
-      <c r="B69" s="133" t="s">
+      <c r="B69" s="134" t="s">
+        <v>271</v>
+      </c>
+      <c r="C69" s="14" t="s">
         <v>272</v>
       </c>
-      <c r="C69" s="14" t="s">
+      <c r="D69" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="D69" s="14" t="s">
+      <c r="E69" s="163"/>
+      <c r="F69" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="E69" s="159"/>
-      <c r="F69" s="14" t="s">
+      <c r="G69" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="G69" s="18" t="s">
+      <c r="H69" s="28" t="s">
         <v>276</v>
       </c>
-      <c r="H69" s="28" t="s">
-        <v>277</v>
-      </c>
-      <c r="I69" s="111"/>
+      <c r="I69" s="112"/>
       <c r="J69" s="1"/>
     </row>
     <row r="70" ht="30.75" customHeight="1" spans="1:10">
       <c r="A70" s="11"/>
-      <c r="B70" s="85"/>
-      <c r="C70" s="75" t="s">
+      <c r="B70" s="86"/>
+      <c r="C70" s="76" t="s">
+        <v>277</v>
+      </c>
+      <c r="D70" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="D70" s="18" t="s">
+      <c r="E70" s="163"/>
+      <c r="F70" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="E70" s="159"/>
-      <c r="F70" s="18" t="s">
+      <c r="G70" s="76" t="s">
         <v>280</v>
       </c>
-      <c r="G70" s="75" t="s">
+      <c r="H70" s="83" t="s">
         <v>281</v>
       </c>
-      <c r="H70" s="82" t="s">
-        <v>282</v>
-      </c>
-      <c r="I70" s="112"/>
+      <c r="I70" s="113"/>
       <c r="J70" s="1"/>
     </row>
     <row r="71" ht="28.5" customHeight="1" spans="1:10">
       <c r="A71" s="11"/>
       <c r="B71" s="17"/>
       <c r="C71" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="D71" s="83" t="s">
         <v>283</v>
       </c>
-      <c r="D71" s="82" t="s">
+      <c r="E71" s="163"/>
+      <c r="F71" s="18" t="s">
         <v>284</v>
       </c>
-      <c r="E71" s="159"/>
-      <c r="F71" s="18" t="s">
+      <c r="G71" s="18" t="s">
         <v>285</v>
       </c>
-      <c r="G71" s="18" t="s">
+      <c r="H71" s="164" t="s">
         <v>286</v>
       </c>
-      <c r="H71" s="160" t="s">
-        <v>287</v>
-      </c>
-      <c r="I71" s="111"/>
+      <c r="I71" s="112"/>
       <c r="J71" s="1"/>
     </row>
     <row r="72" ht="31.5" customHeight="1" spans="1:10">
       <c r="A72" s="11"/>
-      <c r="B72" s="134"/>
-      <c r="C72" s="82" t="s">
+      <c r="B72" s="135"/>
+      <c r="C72" s="83" t="s">
+        <v>287</v>
+      </c>
+      <c r="D72" s="76" t="s">
         <v>288</v>
       </c>
-      <c r="D72" s="75" t="s">
+      <c r="E72" s="163"/>
+      <c r="F72" s="83" t="s">
         <v>289</v>
       </c>
-      <c r="E72" s="159"/>
-      <c r="F72" s="82" t="s">
+      <c r="G72" s="13"/>
+      <c r="H72" s="83" t="s">
         <v>290</v>
       </c>
-      <c r="G72" s="13"/>
-      <c r="H72" s="82" t="s">
-        <v>291</v>
-      </c>
-      <c r="I72" s="111"/>
+      <c r="I72" s="112"/>
       <c r="J72" s="1"/>
     </row>
     <row r="73" ht="36.75" customHeight="1" spans="1:10">
       <c r="A73" s="11"/>
-      <c r="B73" s="85"/>
-      <c r="C73" s="82" t="s">
+      <c r="B73" s="86"/>
+      <c r="C73" s="83" t="s">
+        <v>291</v>
+      </c>
+      <c r="D73" s="18" t="s">
         <v>292</v>
       </c>
-      <c r="D73" s="18" t="s">
+      <c r="E73" s="163"/>
+      <c r="F73" s="83" t="s">
         <v>293</v>
-      </c>
-      <c r="E73" s="159"/>
-      <c r="F73" s="82" t="s">
-        <v>294</v>
       </c>
       <c r="G73" s="29"/>
       <c r="H73" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="I73" s="112"/>
+        <v>294</v>
+      </c>
+      <c r="I73" s="113"/>
       <c r="J73" s="1"/>
     </row>
     <row r="74" ht="27.75" customHeight="1" spans="1:10">
       <c r="A74" s="11"/>
       <c r="B74" s="18"/>
       <c r="C74" s="30" t="s">
+        <v>295</v>
+      </c>
+      <c r="D74" s="30"/>
+      <c r="E74" s="163"/>
+      <c r="F74" s="76" t="s">
         <v>296</v>
-      </c>
-      <c r="D74" s="30"/>
-      <c r="E74" s="159"/>
-      <c r="F74" s="75" t="s">
-        <v>297</v>
       </c>
       <c r="G74" s="18"/>
       <c r="H74" s="20" t="s">
-        <v>298</v>
-      </c>
-      <c r="I74" s="127"/>
+        <v>297</v>
+      </c>
+      <c r="I74" s="128"/>
       <c r="J74" s="1"/>
     </row>
     <row r="75" ht="21" customHeight="1" spans="1:10">
       <c r="A75" s="11"/>
       <c r="B75" s="18"/>
       <c r="C75" s="30" t="s">
+        <v>298</v>
+      </c>
+      <c r="D75" s="30"/>
+      <c r="E75" s="163"/>
+      <c r="F75" s="62" t="s">
         <v>299</v>
-      </c>
-      <c r="D75" s="30"/>
-      <c r="E75" s="159"/>
-      <c r="F75" s="62" t="s">
-        <v>300</v>
       </c>
       <c r="G75" s="62"/>
       <c r="H75" s="62" t="s">
-        <v>301</v>
-      </c>
-      <c r="I75" s="127"/>
+        <v>300</v>
+      </c>
+      <c r="I75" s="128"/>
       <c r="J75" s="1"/>
     </row>
     <row r="76" ht="33" customHeight="1" spans="1:10">
       <c r="A76" s="11"/>
       <c r="B76" s="18"/>
       <c r="C76" s="30" t="s">
+        <v>301</v>
+      </c>
+      <c r="D76" s="30"/>
+      <c r="E76" s="163"/>
+      <c r="F76" s="62" t="s">
         <v>302</v>
-      </c>
-      <c r="D76" s="30"/>
-      <c r="E76" s="159"/>
-      <c r="F76" s="62" t="s">
-        <v>303</v>
       </c>
       <c r="G76" s="62"/>
       <c r="H76" s="62" t="s">
-        <v>304</v>
-      </c>
-      <c r="I76" s="175"/>
+        <v>303</v>
+      </c>
+      <c r="I76" s="179"/>
       <c r="J76" s="1"/>
     </row>
     <row r="77" ht="27.75" customHeight="1" spans="1:10">
       <c r="A77" s="11"/>
       <c r="B77" s="31" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C77" s="31"/>
       <c r="D77" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="E77" s="163"/>
+      <c r="F77" s="77" t="s">
         <v>306</v>
       </c>
-      <c r="E77" s="159"/>
-      <c r="F77" s="76" t="s">
+      <c r="G77" s="77"/>
+      <c r="H77" s="88" t="s">
         <v>307</v>
       </c>
-      <c r="G77" s="76"/>
-      <c r="H77" s="76" t="s">
+      <c r="I77" s="120"/>
+      <c r="J77" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="I77" s="175"/>
-      <c r="J77" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="78" ht="33" customHeight="1" spans="1:10">
       <c r="A78" s="11"/>
       <c r="B78" s="27" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C78" s="31"/>
       <c r="D78" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="E78" s="163"/>
+      <c r="F78" s="77" t="s">
         <v>311</v>
       </c>
-      <c r="E78" s="159"/>
-      <c r="F78" s="76" t="s">
+      <c r="G78" s="77"/>
+      <c r="H78" s="88" t="s">
         <v>312</v>
       </c>
-      <c r="G78" s="76"/>
-      <c r="H78" s="76" t="s">
-        <v>313</v>
-      </c>
-      <c r="I78" s="123"/>
+      <c r="I78" s="120"/>
       <c r="J78" s="1"/>
     </row>
     <row r="79" ht="28.5" customHeight="1" spans="1:10">
       <c r="A79" s="11"/>
-      <c r="B79" s="135" t="s">
+      <c r="B79" s="136" t="s">
+        <v>313</v>
+      </c>
+      <c r="C79" s="137"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="163"/>
+      <c r="F79" s="32" t="s">
         <v>314</v>
-      </c>
-      <c r="C79" s="136"/>
-      <c r="D79" s="29"/>
-      <c r="E79" s="159"/>
-      <c r="F79" s="32" t="s">
-        <v>315</v>
       </c>
       <c r="G79" s="33"/>
       <c r="H79" s="29" t="s">
-        <v>287</v>
-      </c>
-      <c r="I79" s="115"/>
+        <v>286</v>
+      </c>
+      <c r="I79" s="116"/>
       <c r="J79" s="1"/>
     </row>
     <row r="80" ht="18" customHeight="1" spans="1:10">
       <c r="A80" s="11"/>
-      <c r="B80" s="135" t="s">
+      <c r="B80" s="136" t="s">
+        <v>315</v>
+      </c>
+      <c r="C80" s="137"/>
+      <c r="D80" s="14"/>
+      <c r="E80" s="163"/>
+      <c r="F80" s="36" t="s">
         <v>316</v>
       </c>
-      <c r="C80" s="136"/>
-      <c r="D80" s="14"/>
-      <c r="E80" s="159"/>
-      <c r="F80" s="36" t="s">
+      <c r="G80" s="36"/>
+      <c r="H80" s="134" t="s">
         <v>317</v>
       </c>
-      <c r="G80" s="36"/>
-      <c r="H80" s="34"/>
-      <c r="I80" s="176"/>
+      <c r="I80" s="180"/>
       <c r="J80" s="1"/>
     </row>
     <row r="81" ht="27.75" customHeight="1" spans="1:10">
@@ -5838,9 +5849,9 @@
       </c>
       <c r="C81" s="33"/>
       <c r="D81" s="34"/>
-      <c r="E81" s="161"/>
+      <c r="E81" s="165"/>
       <c r="H81" s="36"/>
-      <c r="I81" s="177"/>
+      <c r="I81" s="181"/>
       <c r="J81" s="1"/>
     </row>
     <row r="82" ht="15" spans="1:10">
@@ -5850,25 +5861,25 @@
       </c>
       <c r="C82" s="36"/>
       <c r="D82" s="36"/>
-      <c r="E82" s="159"/>
+      <c r="E82" s="163"/>
       <c r="F82" s="29"/>
       <c r="G82" s="29"/>
-      <c r="I82" s="123"/>
+      <c r="I82" s="124"/>
       <c r="J82" s="1"/>
     </row>
     <row r="83" ht="9" customHeight="1" spans="1:9">
-      <c r="A83" s="137"/>
-      <c r="B83" s="68"/>
-      <c r="C83" s="69"/>
-      <c r="D83" s="69"/>
-      <c r="E83" s="162"/>
-      <c r="F83" s="69"/>
-      <c r="G83" s="69"/>
+      <c r="A83" s="138"/>
+      <c r="B83" s="69"/>
+      <c r="C83" s="70"/>
+      <c r="D83" s="70"/>
+      <c r="E83" s="166"/>
+      <c r="F83" s="70"/>
+      <c r="G83" s="70"/>
       <c r="H83" s="29"/>
-      <c r="I83" s="178"/>
+      <c r="I83" s="182"/>
     </row>
     <row r="84" ht="37.5" customHeight="1" spans="1:9">
-      <c r="A84" s="138" t="s">
+      <c r="A84" s="139" t="s">
         <v>320</v>
       </c>
       <c r="B84" s="12" t="s">
@@ -5880,22 +5891,22 @@
       <c r="D84" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="E84" s="79" t="s">
+      <c r="E84" s="80" t="s">
         <v>13</v>
       </c>
       <c r="F84" s="14" t="s">
         <v>324</v>
       </c>
-      <c r="G84" s="163" t="s">
+      <c r="G84" s="167" t="s">
         <v>325</v>
       </c>
-      <c r="H84" s="69"/>
-      <c r="I84" s="110" t="s">
-        <v>254</v>
+      <c r="H84" s="70"/>
+      <c r="I84" s="111" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="85" ht="44.25" customHeight="1" spans="1:9">
-      <c r="A85" s="139"/>
+      <c r="A85" s="140"/>
       <c r="B85" s="12" t="s">
         <v>326</v>
       </c>
@@ -5905,20 +5916,20 @@
       <c r="D85" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="E85" s="73"/>
+      <c r="E85" s="74"/>
       <c r="F85" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="G85" s="164"/>
+      <c r="G85" s="168"/>
       <c r="H85" s="14" t="s">
         <v>330</v>
       </c>
-      <c r="I85" s="110" t="s">
+      <c r="I85" s="111" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="86" ht="36" customHeight="1" spans="1:9">
-      <c r="A86" s="139"/>
+      <c r="A86" s="140"/>
       <c r="B86" s="12" t="s">
         <v>331</v>
       </c>
@@ -5928,20 +5939,20 @@
       <c r="D86" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="E86" s="73"/>
+      <c r="E86" s="74"/>
       <c r="F86" s="14" t="s">
         <v>334</v>
       </c>
-      <c r="G86" s="164"/>
+      <c r="G86" s="168"/>
       <c r="H86" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="I86" s="110" t="s">
+      <c r="I86" s="111" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="87" ht="30" customHeight="1" spans="1:9">
-      <c r="A87" s="139"/>
+      <c r="A87" s="140"/>
       <c r="B87" s="12" t="s">
         <v>337</v>
       </c>
@@ -5951,19 +5962,19 @@
       <c r="D87" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="E87" s="73"/>
+      <c r="E87" s="74"/>
       <c r="F87" s="14" t="s">
         <v>340</v>
       </c>
-      <c r="G87" s="164"/>
+      <c r="G87" s="168"/>
       <c r="H87" s="14" t="s">
         <v>341</v>
       </c>
-      <c r="I87" s="111"/>
+      <c r="I87" s="112"/>
     </row>
     <row r="88" ht="26.25" customHeight="1" spans="1:9">
-      <c r="A88" s="139"/>
-      <c r="B88" s="134" t="s">
+      <c r="A88" s="140"/>
+      <c r="B88" s="135" t="s">
         <v>342</v>
       </c>
       <c r="C88" s="14" t="s">
@@ -5972,60 +5983,60 @@
       <c r="D88" s="14" t="s">
         <v>344</v>
       </c>
-      <c r="E88" s="73"/>
+      <c r="E88" s="74"/>
       <c r="F88" s="18" t="s">
         <v>345</v>
       </c>
-      <c r="G88" s="164"/>
-      <c r="H88" s="75" t="s">
+      <c r="G88" s="168"/>
+      <c r="H88" s="76" t="s">
         <v>346</v>
       </c>
-      <c r="I88" s="111"/>
+      <c r="I88" s="112"/>
     </row>
     <row r="89" ht="36" customHeight="1" spans="1:9">
-      <c r="A89" s="139"/>
-      <c r="B89" s="134" t="s">
+      <c r="A89" s="140"/>
+      <c r="B89" s="135" t="s">
         <v>347</v>
       </c>
       <c r="C89" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D89" s="14" t="s">
         <v>348</v>
       </c>
-      <c r="E89" s="73"/>
+      <c r="E89" s="74"/>
       <c r="F89" s="13" t="s">
         <v>349</v>
       </c>
-      <c r="G89" s="164"/>
+      <c r="G89" s="168"/>
       <c r="H89" s="22" t="s">
         <v>350</v>
       </c>
-      <c r="I89" s="111"/>
+      <c r="I89" s="112"/>
     </row>
     <row r="90" ht="39.75" customHeight="1" spans="1:9">
-      <c r="A90" s="139"/>
+      <c r="A90" s="140"/>
       <c r="B90" s="55" t="s">
         <v>351</v>
       </c>
-      <c r="C90" s="82" t="s">
+      <c r="C90" s="83" t="s">
         <v>352</v>
       </c>
       <c r="D90" s="18" t="s">
         <v>353</v>
       </c>
-      <c r="E90" s="73"/>
+      <c r="E90" s="74"/>
       <c r="F90" s="13" t="s">
         <v>354</v>
       </c>
-      <c r="G90" s="164"/>
-      <c r="H90" s="75" t="s">
+      <c r="G90" s="168"/>
+      <c r="H90" s="76" t="s">
         <v>355</v>
       </c>
-      <c r="I90" s="111"/>
+      <c r="I90" s="112"/>
     </row>
     <row r="91" ht="33.75" customHeight="1" spans="1:9">
-      <c r="A91" s="139"/>
+      <c r="A91" s="140"/>
       <c r="B91" s="29"/>
       <c r="C91" s="20" t="s">
         <v>356</v>
@@ -6033,18 +6044,18 @@
       <c r="D91" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="E91" s="73"/>
-      <c r="F91" s="165" t="s">
+      <c r="E91" s="74"/>
+      <c r="F91" s="169" t="s">
         <v>358</v>
       </c>
-      <c r="G91" s="164"/>
-      <c r="H91" s="75" t="s">
+      <c r="G91" s="168"/>
+      <c r="H91" s="76" t="s">
         <v>359</v>
       </c>
-      <c r="I91" s="111"/>
+      <c r="I91" s="112"/>
     </row>
     <row r="92" ht="39" customHeight="1" spans="1:9">
-      <c r="A92" s="139"/>
+      <c r="A92" s="140"/>
       <c r="B92" s="29"/>
       <c r="C92" s="18" t="s">
         <v>360</v>
@@ -6052,303 +6063,305 @@
       <c r="D92" s="18" t="s">
         <v>361</v>
       </c>
-      <c r="E92" s="73"/>
-      <c r="F92" s="166"/>
-      <c r="G92" s="164"/>
-      <c r="H92" s="82" t="s">
+      <c r="E92" s="74"/>
+      <c r="F92" s="170"/>
+      <c r="G92" s="168"/>
+      <c r="H92" s="83" t="s">
         <v>362</v>
       </c>
-      <c r="I92" s="111"/>
+      <c r="I92" s="112"/>
     </row>
     <row r="93" ht="32.25" customHeight="1" spans="1:9">
-      <c r="A93" s="139"/>
+      <c r="A93" s="140"/>
       <c r="B93" s="17"/>
       <c r="C93" s="18" t="s">
         <v>363</v>
       </c>
       <c r="D93" s="18"/>
-      <c r="E93" s="73"/>
-      <c r="F93" s="166"/>
-      <c r="G93" s="164"/>
+      <c r="E93" s="74"/>
+      <c r="F93" s="170"/>
+      <c r="G93" s="168"/>
       <c r="H93" s="20" t="s">
         <v>364</v>
       </c>
-      <c r="I93" s="111"/>
+      <c r="I93" s="112"/>
     </row>
     <row r="94" ht="40.5" customHeight="1" spans="1:9">
-      <c r="A94" s="139"/>
-      <c r="B94" s="140" t="s">
+      <c r="A94" s="140"/>
+      <c r="B94" s="141" t="s">
         <v>365</v>
       </c>
-      <c r="C94" s="141"/>
+      <c r="C94" s="142"/>
       <c r="D94" s="18"/>
-      <c r="E94" s="73"/>
+      <c r="E94" s="74"/>
       <c r="F94" s="18"/>
-      <c r="G94" s="164"/>
+      <c r="G94" s="168"/>
       <c r="H94" s="20" t="s">
         <v>366</v>
       </c>
-      <c r="I94" s="111"/>
+      <c r="I94" s="112"/>
     </row>
     <row r="95" ht="32.25" customHeight="1" spans="1:9">
-      <c r="A95" s="139"/>
+      <c r="A95" s="140"/>
       <c r="B95" s="17"/>
-      <c r="C95" s="142" t="s">
+      <c r="C95" s="143" t="s">
         <v>367</v>
       </c>
-      <c r="D95" s="141"/>
-      <c r="E95" s="73"/>
+      <c r="D95" s="142"/>
+      <c r="E95" s="74"/>
       <c r="F95" s="46"/>
-      <c r="G95" s="164"/>
+      <c r="G95" s="168"/>
       <c r="H95" s="20" t="s">
         <v>368</v>
       </c>
-      <c r="I95" s="175"/>
+      <c r="I95" s="179"/>
     </row>
     <row r="96" ht="27.75" customHeight="1" spans="1:9">
-      <c r="A96" s="139"/>
+      <c r="A96" s="140"/>
       <c r="B96" s="12"/>
-      <c r="C96" s="18"/>
+      <c r="C96" s="144" t="s">
+        <v>369</v>
+      </c>
       <c r="D96" s="18"/>
-      <c r="E96" s="73"/>
+      <c r="E96" s="74"/>
       <c r="F96" s="18"/>
-      <c r="G96" s="164"/>
-      <c r="H96" s="76" t="s">
-        <v>369</v>
-      </c>
-      <c r="I96" s="175"/>
+      <c r="G96" s="168"/>
+      <c r="H96" s="77" t="s">
+        <v>370</v>
+      </c>
+      <c r="I96" s="179"/>
     </row>
     <row r="97" ht="23.25" customHeight="1" spans="1:9">
-      <c r="A97" s="139"/>
-      <c r="B97" s="26" t="s">
-        <v>370</v>
-      </c>
-      <c r="C97" s="27"/>
+      <c r="A97" s="140"/>
+      <c r="B97" s="145" t="s">
+        <v>371</v>
+      </c>
+      <c r="C97" s="146"/>
       <c r="D97" s="14"/>
-      <c r="E97" s="73"/>
+      <c r="E97" s="74"/>
       <c r="F97" s="18"/>
-      <c r="G97" s="164"/>
-      <c r="H97" s="76" t="s">
-        <v>371</v>
-      </c>
-      <c r="I97" s="127"/>
+      <c r="G97" s="168"/>
+      <c r="H97" s="77" t="s">
+        <v>372</v>
+      </c>
+      <c r="I97" s="128"/>
     </row>
     <row r="98" ht="20.25" customHeight="1" spans="1:9">
-      <c r="A98" s="139"/>
-      <c r="B98" s="26" t="s">
-        <v>372</v>
-      </c>
-      <c r="C98" s="27"/>
+      <c r="A98" s="140"/>
+      <c r="B98" s="145" t="s">
+        <v>373</v>
+      </c>
+      <c r="C98" s="146"/>
       <c r="D98" s="14"/>
-      <c r="E98" s="73"/>
+      <c r="E98" s="74"/>
       <c r="F98" s="14"/>
-      <c r="G98" s="164"/>
+      <c r="G98" s="168"/>
       <c r="H98" s="62" t="s">
-        <v>373</v>
-      </c>
-      <c r="I98" s="127"/>
+        <v>374</v>
+      </c>
+      <c r="I98" s="128"/>
     </row>
     <row r="99" ht="24" customHeight="1" spans="1:9">
-      <c r="A99" s="139"/>
-      <c r="B99" s="67"/>
+      <c r="A99" s="140"/>
+      <c r="B99" s="68"/>
       <c r="C99" s="30" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="D99" s="30"/>
-      <c r="E99" s="73"/>
+      <c r="E99" s="74"/>
       <c r="F99" s="18"/>
-      <c r="G99" s="164"/>
+      <c r="G99" s="168"/>
       <c r="H99" s="62" t="s">
-        <v>375</v>
-      </c>
-      <c r="I99" s="175"/>
+        <v>376</v>
+      </c>
+      <c r="I99" s="179"/>
     </row>
     <row r="100" ht="37.5" customHeight="1" spans="1:9">
-      <c r="A100" s="139"/>
+      <c r="A100" s="140"/>
       <c r="B100" s="12"/>
       <c r="C100" s="30" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D100" s="30"/>
-      <c r="E100" s="73"/>
-      <c r="F100" s="166"/>
-      <c r="G100" s="164"/>
-      <c r="H100" s="76" t="s">
-        <v>377</v>
-      </c>
-      <c r="I100" s="175"/>
+      <c r="E100" s="74"/>
+      <c r="F100" s="170"/>
+      <c r="G100" s="168"/>
+      <c r="H100" s="77" t="s">
+        <v>378</v>
+      </c>
+      <c r="I100" s="179"/>
     </row>
     <row r="101" ht="18.75" customHeight="1" spans="1:9">
-      <c r="A101" s="139"/>
-      <c r="B101" s="67"/>
+      <c r="A101" s="140"/>
+      <c r="B101" s="68"/>
       <c r="C101" s="62"/>
       <c r="D101" s="62"/>
-      <c r="E101" s="73"/>
-      <c r="F101" s="166"/>
-      <c r="G101" s="164"/>
-      <c r="H101" s="76" t="s">
-        <v>378</v>
-      </c>
-      <c r="I101" s="113"/>
+      <c r="E101" s="74"/>
+      <c r="F101" s="170"/>
+      <c r="G101" s="168"/>
+      <c r="H101" s="77" t="s">
+        <v>379</v>
+      </c>
+      <c r="I101" s="114"/>
     </row>
     <row r="102" ht="19.5" customHeight="1" spans="1:9">
-      <c r="A102" s="139"/>
+      <c r="A102" s="140"/>
       <c r="B102" s="32" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C102" s="33"/>
       <c r="D102" s="34"/>
-      <c r="E102" s="73"/>
-      <c r="F102" s="166"/>
-      <c r="G102" s="167"/>
+      <c r="E102" s="74"/>
+      <c r="F102" s="170"/>
+      <c r="G102" s="171"/>
       <c r="H102" s="31" t="s">
-        <v>380</v>
-      </c>
-      <c r="I102" s="113"/>
+        <v>381</v>
+      </c>
+      <c r="I102" s="114"/>
     </row>
     <row r="103" ht="17.25" customHeight="1" spans="1:9">
-      <c r="A103" s="139"/>
+      <c r="A103" s="140"/>
       <c r="B103" s="36" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C103" s="36"/>
       <c r="D103" s="36"/>
-      <c r="E103" s="168"/>
-      <c r="G103" s="169" t="s">
-        <v>382</v>
+      <c r="E103" s="172"/>
+      <c r="G103" s="173" t="s">
+        <v>383</v>
       </c>
       <c r="H103" s="31" t="s">
-        <v>383</v>
-      </c>
-      <c r="I103" s="102"/>
+        <v>384</v>
+      </c>
+      <c r="I103" s="103"/>
     </row>
     <row r="104" ht="19.5" customHeight="1" spans="1:9">
-      <c r="A104" s="143"/>
+      <c r="A104" s="147"/>
       <c r="B104" s="38" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C104" s="38"/>
       <c r="D104" s="38"/>
-      <c r="E104" s="73"/>
+      <c r="E104" s="74"/>
       <c r="F104" s="10"/>
       <c r="G104" s="36" t="s">
-        <v>385</v>
-      </c>
-      <c r="H104" s="102"/>
+        <v>386</v>
+      </c>
+      <c r="H104" s="103"/>
       <c r="I104" s="36"/>
     </row>
     <row r="105" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A105" s="144"/>
+      <c r="A105" s="148"/>
       <c r="B105" s="18"/>
       <c r="C105" s="31"/>
       <c r="D105" s="31"/>
-      <c r="E105" s="91"/>
+      <c r="E105" s="92"/>
       <c r="F105" s="14"/>
       <c r="G105" s="36" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H105" s="36"/>
       <c r="I105" s="36"/>
     </row>
     <row r="106" ht="11.25" customHeight="1" spans="1:9">
-      <c r="A106" s="145"/>
-      <c r="B106" s="68"/>
-      <c r="C106" s="69"/>
-      <c r="D106" s="69"/>
-      <c r="E106" s="170"/>
-      <c r="F106" s="69"/>
-      <c r="G106" s="69"/>
+      <c r="A106" s="149"/>
+      <c r="B106" s="69"/>
+      <c r="C106" s="70"/>
+      <c r="D106" s="70"/>
+      <c r="E106" s="174"/>
+      <c r="F106" s="70"/>
+      <c r="G106" s="70"/>
       <c r="H106" s="36"/>
-      <c r="I106" s="178"/>
+      <c r="I106" s="182"/>
     </row>
     <row r="107" ht="33.75" customHeight="1" spans="1:9">
       <c r="A107" s="8" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B107" s="17" t="s">
         <v>93</v>
       </c>
       <c r="C107" s="14" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D107" s="14" t="s">
         <v>97</v>
       </c>
       <c r="E107" s="46" t="s">
-        <v>389</v>
-      </c>
-      <c r="F107" s="67"/>
-      <c r="G107" s="171"/>
-      <c r="H107" s="69"/>
-      <c r="I107" s="179"/>
+        <v>390</v>
+      </c>
+      <c r="F107" s="68"/>
+      <c r="G107" s="175"/>
+      <c r="H107" s="70"/>
+      <c r="I107" s="183"/>
     </row>
     <row r="108" ht="33.75" customHeight="1" spans="1:9">
-      <c r="A108" s="146"/>
+      <c r="A108" s="150"/>
       <c r="B108" s="12" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="D108" s="14" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="E108" s="46" t="s">
-        <v>393</v>
-      </c>
-      <c r="F108" s="67"/>
-      <c r="G108" s="172"/>
-      <c r="H108" s="171"/>
-      <c r="I108" s="109"/>
+        <v>394</v>
+      </c>
+      <c r="F108" s="68"/>
+      <c r="G108" s="176"/>
+      <c r="H108" s="175"/>
+      <c r="I108" s="110"/>
     </row>
     <row r="109" ht="33.75" customHeight="1" spans="1:9">
-      <c r="A109" s="146"/>
+      <c r="A109" s="150"/>
       <c r="B109" s="12" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C109" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="D109" s="74" t="s">
-        <v>395</v>
+      <c r="D109" s="75" t="s">
+        <v>396</v>
       </c>
       <c r="E109" s="62"/>
-      <c r="F109" s="67"/>
-      <c r="G109" s="172"/>
-      <c r="H109" s="172"/>
-      <c r="I109" s="109"/>
+      <c r="F109" s="68"/>
+      <c r="G109" s="176"/>
+      <c r="H109" s="176"/>
+      <c r="I109" s="110"/>
     </row>
     <row r="110" ht="33.75" customHeight="1" spans="1:9">
       <c r="A110" s="11"/>
       <c r="B110" s="12"/>
       <c r="C110" s="18" t="s">
-        <v>396</v>
-      </c>
-      <c r="D110" s="100" t="s">
         <v>397</v>
       </c>
-      <c r="E110" s="100"/>
+      <c r="D110" s="101" t="s">
+        <v>398</v>
+      </c>
+      <c r="E110" s="101"/>
       <c r="F110" s="17"/>
       <c r="G110" s="18"/>
-      <c r="H110" s="172"/>
-      <c r="I110" s="110"/>
+      <c r="H110" s="176"/>
+      <c r="I110" s="111"/>
     </row>
     <row r="111" ht="33.75" customHeight="1" spans="1:9">
       <c r="A111" s="11"/>
       <c r="B111" s="17" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C111" s="25" t="s">
-        <v>399</v>
-      </c>
-      <c r="D111" s="100" t="s">
         <v>400</v>
       </c>
-      <c r="E111" s="100"/>
+      <c r="D111" s="101" t="s">
+        <v>401</v>
+      </c>
+      <c r="E111" s="101"/>
       <c r="F111" s="17"/>
       <c r="G111" s="18"/>
       <c r="H111" s="18"/>
-      <c r="I111" s="110"/>
+      <c r="I111" s="111"/>
     </row>
     <row r="112" ht="33.75" customHeight="1" spans="1:9">
       <c r="A112" s="11"/>
@@ -6359,119 +6372,119 @@
       <c r="F112" s="17"/>
       <c r="G112" s="18"/>
       <c r="H112" s="18"/>
-      <c r="I112" s="110"/>
+      <c r="I112" s="111"/>
     </row>
     <row r="113" ht="25.5" customHeight="1" spans="1:9">
       <c r="A113" s="11"/>
       <c r="B113" s="17"/>
       <c r="C113" s="30" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D113" s="30"/>
       <c r="E113" s="18"/>
       <c r="F113" s="17"/>
       <c r="G113" s="18"/>
       <c r="H113" s="18"/>
-      <c r="I113" s="110"/>
+      <c r="I113" s="111"/>
     </row>
     <row r="114" ht="24.75" customHeight="1" spans="1:9">
       <c r="A114" s="11"/>
       <c r="B114" s="17"/>
       <c r="C114" s="30" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="D114" s="30"/>
       <c r="E114" s="18"/>
       <c r="F114" s="17"/>
       <c r="G114" s="18"/>
       <c r="H114" s="18"/>
-      <c r="I114" s="110"/>
+      <c r="I114" s="111"/>
     </row>
     <row r="115" ht="24.75" customHeight="1" spans="1:9">
       <c r="A115" s="11"/>
       <c r="B115" s="17"/>
-      <c r="C115" s="100" t="s">
-        <v>403</v>
-      </c>
-      <c r="D115" s="100"/>
+      <c r="C115" s="101" t="s">
+        <v>404</v>
+      </c>
+      <c r="D115" s="101"/>
       <c r="E115" s="18"/>
       <c r="F115" s="17"/>
       <c r="G115" s="18"/>
       <c r="H115" s="18"/>
-      <c r="I115" s="110"/>
+      <c r="I115" s="111"/>
     </row>
     <row r="116" ht="36.75" customHeight="1" spans="1:9">
       <c r="A116" s="11"/>
       <c r="B116" s="27" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C116" s="31"/>
       <c r="D116" s="30" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="E116" s="30"/>
       <c r="F116" s="17"/>
       <c r="G116" s="18"/>
       <c r="H116" s="18"/>
-      <c r="I116" s="110"/>
+      <c r="I116" s="111"/>
     </row>
     <row r="117" ht="27" customHeight="1" spans="1:9">
       <c r="A117" s="11"/>
       <c r="B117" s="27" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C117" s="31"/>
       <c r="D117" s="31" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="E117" s="31"/>
-      <c r="F117" s="67"/>
+      <c r="F117" s="68"/>
       <c r="G117" s="18"/>
       <c r="H117" s="18"/>
-      <c r="I117" s="110"/>
+      <c r="I117" s="111"/>
     </row>
     <row r="118" ht="21.75" customHeight="1" spans="1:9">
       <c r="A118" s="11"/>
       <c r="B118" s="27" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C118" s="31"/>
       <c r="D118" s="31" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="E118" s="31"/>
       <c r="F118" s="29"/>
       <c r="G118" s="18"/>
       <c r="H118" s="18"/>
-      <c r="I118" s="110"/>
+      <c r="I118" s="111"/>
     </row>
     <row r="119" ht="22.5" customHeight="1" spans="1:9">
       <c r="A119" s="11"/>
       <c r="B119" s="27" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C119" s="31"/>
       <c r="F119" s="12"/>
       <c r="G119" s="18"/>
       <c r="H119" s="18"/>
-      <c r="I119" s="110"/>
+      <c r="I119" s="111"/>
     </row>
     <row r="120" ht="26.25" customHeight="1" spans="1:9">
       <c r="A120" s="11"/>
       <c r="B120" s="32" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C120" s="33"/>
       <c r="D120" s="34"/>
       <c r="F120" s="12"/>
       <c r="G120" s="18"/>
       <c r="H120" s="18"/>
-      <c r="I120" s="110"/>
+      <c r="I120" s="111"/>
     </row>
     <row r="121" customHeight="1" spans="1:9">
       <c r="A121" s="11"/>
       <c r="B121" s="36" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C121" s="36"/>
       <c r="D121" s="36"/>
@@ -6479,12 +6492,12 @@
       <c r="F121" s="17"/>
       <c r="G121" s="18"/>
       <c r="H121" s="18"/>
-      <c r="I121" s="110"/>
+      <c r="I121" s="111"/>
     </row>
     <row r="122" ht="17.25" customHeight="1" spans="1:9">
       <c r="A122" s="11"/>
       <c r="B122" s="38" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C122" s="38"/>
       <c r="D122" s="38"/>
@@ -6492,7 +6505,7 @@
       <c r="F122" s="12"/>
       <c r="G122" s="18"/>
       <c r="H122" s="18"/>
-      <c r="I122" s="110"/>
+      <c r="I122" s="111"/>
     </row>
     <row r="123" ht="15" spans="1:9">
       <c r="A123" s="39"/>
@@ -6503,708 +6516,766 @@
       <c r="F123" s="12"/>
       <c r="G123" s="18"/>
       <c r="H123" s="18"/>
-      <c r="I123" s="110"/>
+      <c r="I123" s="111"/>
     </row>
     <row r="124" s="1" customFormat="1" ht="6.75" customHeight="1" spans="1:9">
-      <c r="A124" s="147"/>
-      <c r="B124" s="148"/>
-      <c r="C124" s="149"/>
-      <c r="D124" s="149"/>
-      <c r="E124" s="173"/>
-      <c r="F124" s="149"/>
-      <c r="G124" s="149"/>
+      <c r="A124" s="151"/>
+      <c r="B124" s="152"/>
+      <c r="C124" s="153"/>
+      <c r="D124" s="153"/>
+      <c r="E124" s="177"/>
+      <c r="F124" s="153"/>
+      <c r="G124" s="153"/>
       <c r="H124" s="18"/>
-      <c r="I124" s="180"/>
+      <c r="I124" s="184"/>
     </row>
     <row r="125" ht="15" spans="1:9">
-      <c r="A125" s="150">
+      <c r="A125" s="154">
         <v>1</v>
       </c>
-      <c r="B125" s="151" t="s">
-        <v>414</v>
-      </c>
-      <c r="C125" s="152"/>
-      <c r="D125" s="152"/>
-      <c r="E125" s="152"/>
-      <c r="F125" s="152"/>
-      <c r="G125" s="152"/>
-      <c r="H125" s="149"/>
-      <c r="I125" s="181"/>
+      <c r="B125" s="155" t="s">
+        <v>415</v>
+      </c>
+      <c r="C125" s="156"/>
+      <c r="D125" s="156"/>
+      <c r="E125" s="156"/>
+      <c r="F125" s="156"/>
+      <c r="G125" s="156"/>
+      <c r="H125" s="153"/>
+      <c r="I125" s="185"/>
     </row>
     <row r="126" spans="1:9">
-      <c r="A126" s="153"/>
-      <c r="B126" s="154" t="s">
-        <v>415</v>
-      </c>
-      <c r="C126" s="155"/>
-      <c r="D126" s="155"/>
-      <c r="E126" s="155"/>
-      <c r="F126" s="155"/>
-      <c r="G126" s="155"/>
-      <c r="H126" s="152"/>
-      <c r="I126" s="182"/>
+      <c r="A126" s="157"/>
+      <c r="B126" s="158" t="s">
+        <v>416</v>
+      </c>
+      <c r="C126" s="159"/>
+      <c r="D126" s="159"/>
+      <c r="E126" s="159"/>
+      <c r="F126" s="159"/>
+      <c r="G126" s="159"/>
+      <c r="H126" s="156"/>
+      <c r="I126" s="186"/>
     </row>
     <row r="127" customHeight="1" spans="1:9">
-      <c r="A127" s="153"/>
-      <c r="B127" s="156" t="s">
-        <v>416</v>
-      </c>
-      <c r="C127" s="157"/>
-      <c r="D127" s="157"/>
-      <c r="E127" s="157"/>
-      <c r="F127" s="157"/>
-      <c r="G127" s="157"/>
-      <c r="H127" s="155"/>
-      <c r="I127" s="183"/>
+      <c r="A127" s="157"/>
+      <c r="B127" s="160" t="s">
+        <v>417</v>
+      </c>
+      <c r="C127" s="161"/>
+      <c r="D127" s="161"/>
+      <c r="E127" s="161"/>
+      <c r="F127" s="161"/>
+      <c r="G127" s="161"/>
+      <c r="H127" s="159"/>
+      <c r="I127" s="187"/>
     </row>
     <row r="128" customHeight="1" spans="1:9">
-      <c r="A128" s="153"/>
-      <c r="B128" s="156" t="s">
-        <v>417</v>
-      </c>
-      <c r="C128" s="157"/>
-      <c r="D128" s="157"/>
-      <c r="E128" s="157"/>
-      <c r="F128" s="157"/>
-      <c r="G128" s="157"/>
-      <c r="H128" s="157"/>
-      <c r="I128" s="183"/>
+      <c r="A128" s="157"/>
+      <c r="B128" s="160" t="s">
+        <v>418</v>
+      </c>
+      <c r="C128" s="161"/>
+      <c r="D128" s="161"/>
+      <c r="E128" s="161"/>
+      <c r="F128" s="161"/>
+      <c r="G128" s="161"/>
+      <c r="H128" s="161"/>
+      <c r="I128" s="187"/>
     </row>
     <row r="129" spans="1:9">
-      <c r="A129" s="153"/>
-      <c r="B129" s="156" t="s">
-        <v>418</v>
-      </c>
-      <c r="C129" s="157"/>
-      <c r="D129" s="157"/>
-      <c r="E129" s="157"/>
-      <c r="F129" s="157"/>
-      <c r="G129" s="157"/>
-      <c r="H129" s="157"/>
-      <c r="I129" s="183"/>
+      <c r="A129" s="157"/>
+      <c r="B129" s="160" t="s">
+        <v>419</v>
+      </c>
+      <c r="C129" s="161"/>
+      <c r="D129" s="161"/>
+      <c r="E129" s="161"/>
+      <c r="F129" s="161"/>
+      <c r="G129" s="161"/>
+      <c r="H129" s="161"/>
+      <c r="I129" s="187"/>
     </row>
     <row r="130" ht="15" spans="1:9">
-      <c r="A130" s="184"/>
-      <c r="B130" s="185" t="s">
-        <v>419</v>
-      </c>
-      <c r="C130" s="186"/>
-      <c r="D130" s="186"/>
-      <c r="E130" s="186"/>
-      <c r="F130" s="186"/>
-      <c r="G130" s="186"/>
-      <c r="H130" s="157"/>
-      <c r="I130" s="229"/>
+      <c r="A130" s="188"/>
+      <c r="B130" s="189" t="s">
+        <v>420</v>
+      </c>
+      <c r="C130" s="190"/>
+      <c r="D130" s="190"/>
+      <c r="E130" s="190"/>
+      <c r="F130" s="190"/>
+      <c r="G130" s="190"/>
+      <c r="H130" s="161"/>
+      <c r="I130" s="235"/>
     </row>
     <row r="131" spans="1:9">
-      <c r="A131" s="187">
+      <c r="A131" s="191">
         <v>2</v>
       </c>
-      <c r="B131" s="151" t="s">
-        <v>420</v>
-      </c>
-      <c r="C131" s="152"/>
-      <c r="D131" s="152"/>
-      <c r="E131" s="152"/>
-      <c r="F131" s="152"/>
-      <c r="G131" s="152"/>
-      <c r="H131" s="186"/>
-      <c r="I131" s="230"/>
+      <c r="B131" s="155" t="s">
+        <v>421</v>
+      </c>
+      <c r="C131" s="156"/>
+      <c r="D131" s="156"/>
+      <c r="E131" s="156"/>
+      <c r="F131" s="156"/>
+      <c r="G131" s="156"/>
+      <c r="H131" s="190"/>
+      <c r="I131" s="236"/>
     </row>
     <row r="132" customHeight="1" spans="1:8">
-      <c r="A132" s="188"/>
-      <c r="B132" s="189" t="s">
-        <v>421</v>
-      </c>
-      <c r="C132" s="190" t="s">
+      <c r="A132" s="192"/>
+      <c r="B132" s="193" t="s">
         <v>422</v>
       </c>
-      <c r="D132" s="191" t="s">
+      <c r="C132" s="194" t="s">
         <v>423</v>
       </c>
-      <c r="E132" s="219" t="s">
+      <c r="D132" s="195" t="s">
         <v>424</v>
       </c>
-      <c r="F132" s="219" t="s">
+      <c r="E132" s="223" t="s">
         <v>425</v>
       </c>
-      <c r="G132" s="219"/>
-      <c r="H132" s="220"/>
+      <c r="F132" s="223" t="s">
+        <v>426</v>
+      </c>
+      <c r="G132" s="223"/>
+      <c r="H132" s="224"/>
     </row>
     <row r="133" ht="32.25" customHeight="1" spans="1:9">
-      <c r="A133" s="192"/>
-      <c r="B133" s="193"/>
-      <c r="C133" s="194" t="s">
-        <v>426</v>
-      </c>
-      <c r="D133" s="195" t="s">
+      <c r="A133" s="196"/>
+      <c r="B133" s="197"/>
+      <c r="C133" s="198" t="s">
         <v>427</v>
       </c>
-      <c r="E133" s="221"/>
-      <c r="F133" s="221"/>
-      <c r="G133" s="221"/>
-      <c r="H133" s="222" t="s">
+      <c r="D133" s="199" t="s">
         <v>428</v>
       </c>
-      <c r="I133" s="231" t="s">
+      <c r="E133" s="225"/>
+      <c r="F133" s="225"/>
+      <c r="G133" s="225"/>
+      <c r="H133" s="226" t="s">
         <v>429</v>
       </c>
+      <c r="I133" s="237" t="s">
+        <v>430</v>
+      </c>
     </row>
     <row r="134" ht="30.75" spans="1:9">
-      <c r="A134" s="196">
+      <c r="A134" s="200">
         <v>3</v>
       </c>
-      <c r="B134" s="197" t="s">
-        <v>430</v>
-      </c>
-      <c r="C134" s="152" t="s">
-        <v>430</v>
-      </c>
-      <c r="D134" s="152" t="s">
-        <v>430</v>
-      </c>
-      <c r="E134" s="152" t="s">
-        <v>430</v>
-      </c>
-      <c r="F134" s="152" t="s">
-        <v>430</v>
-      </c>
-      <c r="G134" s="152" t="s">
-        <v>430</v>
-      </c>
-      <c r="H134" s="223" t="s">
+      <c r="B134" s="201" t="s">
         <v>431</v>
       </c>
-      <c r="I134" s="232" t="s">
+      <c r="C134" s="156" t="s">
+        <v>431</v>
+      </c>
+      <c r="D134" s="156" t="s">
+        <v>431</v>
+      </c>
+      <c r="E134" s="156" t="s">
+        <v>431</v>
+      </c>
+      <c r="F134" s="156" t="s">
+        <v>431</v>
+      </c>
+      <c r="G134" s="156" t="s">
+        <v>431</v>
+      </c>
+      <c r="H134" s="227" t="s">
         <v>432</v>
       </c>
+      <c r="I134" s="238" t="s">
+        <v>433</v>
+      </c>
     </row>
     <row r="135" ht="15" customHeight="1" spans="1:9">
-      <c r="A135" s="198"/>
-      <c r="B135" s="199"/>
-      <c r="C135" s="157"/>
-      <c r="D135" s="157"/>
-      <c r="E135" s="157"/>
-      <c r="F135" s="157"/>
-      <c r="G135" s="157"/>
-      <c r="H135" s="224" t="s">
-        <v>433</v>
-      </c>
-      <c r="I135" s="233" t="s">
+      <c r="A135" s="202"/>
+      <c r="B135" s="203"/>
+      <c r="C135" s="161"/>
+      <c r="D135" s="161"/>
+      <c r="E135" s="161"/>
+      <c r="F135" s="161"/>
+      <c r="G135" s="161"/>
+      <c r="H135" s="228" t="s">
         <v>434</v>
       </c>
+      <c r="I135" s="239" t="s">
+        <v>435</v>
+      </c>
     </row>
     <row r="136" ht="15" customHeight="1" spans="1:9">
-      <c r="A136" s="198"/>
-      <c r="B136" s="200" t="s">
-        <v>435</v>
-      </c>
-      <c r="C136" s="201" t="s">
+      <c r="A136" s="202"/>
+      <c r="B136" s="204" t="s">
         <v>436</v>
       </c>
-      <c r="D136" s="202" t="s">
+      <c r="C136" s="205" t="s">
         <v>437</v>
       </c>
-      <c r="E136" s="202" t="s">
+      <c r="D136" s="206" t="s">
         <v>438</v>
       </c>
-      <c r="F136" s="213" t="s">
+      <c r="E136" s="206" t="s">
         <v>439</v>
       </c>
-      <c r="G136" s="211" t="s">
+      <c r="F136" s="217" t="s">
         <v>440</v>
       </c>
-      <c r="H136" s="225" t="s">
+      <c r="G136" s="215" t="s">
         <v>441</v>
       </c>
-      <c r="I136" s="234" t="s">
+      <c r="H136" s="229" t="s">
         <v>442</v>
       </c>
+      <c r="I136" s="240" t="s">
+        <v>443</v>
+      </c>
     </row>
     <row r="137" ht="28.5" spans="1:9">
-      <c r="A137" s="198"/>
-      <c r="B137" s="203" t="s">
-        <v>443</v>
-      </c>
-      <c r="C137" s="204" t="s">
+      <c r="A137" s="202"/>
+      <c r="B137" s="207" t="s">
         <v>444</v>
       </c>
-      <c r="D137" s="205" t="s">
+      <c r="C137" s="208" t="s">
         <v>445</v>
       </c>
-      <c r="E137" s="205" t="s">
+      <c r="D137" s="209" t="s">
         <v>446</v>
       </c>
-      <c r="F137" s="226" t="s">
+      <c r="E137" s="209" t="s">
         <v>447</v>
       </c>
-      <c r="G137" s="226" t="s">
+      <c r="F137" s="230" t="s">
         <v>448</v>
       </c>
-      <c r="H137" s="225" t="s">
+      <c r="G137" s="230" t="s">
         <v>449</v>
       </c>
-      <c r="I137" s="234" t="s">
+      <c r="H137" s="229" t="s">
         <v>450</v>
       </c>
+      <c r="I137" s="240" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="138" ht="16.5" spans="1:9">
-      <c r="A138" s="198"/>
-      <c r="B138" s="206" t="s">
-        <v>451</v>
-      </c>
-      <c r="C138" s="207" t="s">
+      <c r="A138" s="202"/>
+      <c r="B138" s="210" t="s">
         <v>452</v>
       </c>
-      <c r="D138" s="208" t="s">
+      <c r="C138" s="211" t="s">
         <v>453</v>
       </c>
-      <c r="E138" s="208" t="s">
+      <c r="D138" s="212" t="s">
         <v>454</v>
       </c>
-      <c r="F138" s="213" t="s">
+      <c r="E138" s="212" t="s">
         <v>455</v>
       </c>
-      <c r="G138" s="213" t="s">
+      <c r="F138" s="217" t="s">
         <v>456</v>
       </c>
-      <c r="H138" s="225" t="s">
+      <c r="G138" s="217" t="s">
         <v>457</v>
       </c>
-      <c r="I138" s="235" t="s">
+      <c r="H138" s="229" t="s">
         <v>458</v>
       </c>
+      <c r="I138" s="241" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="139" ht="16.5" spans="1:9">
-      <c r="A139" s="198"/>
-      <c r="B139" s="206" t="s">
-        <v>459</v>
-      </c>
-      <c r="C139" s="207" t="s">
+      <c r="A139" s="202"/>
+      <c r="B139" s="210" t="s">
         <v>460</v>
       </c>
-      <c r="D139" s="208" t="s">
-        <v>452</v>
-      </c>
-      <c r="E139" s="208" t="s">
+      <c r="C139" s="211" t="s">
         <v>461</v>
       </c>
-      <c r="F139" s="213" t="s">
+      <c r="D139" s="212" t="s">
+        <v>453</v>
+      </c>
+      <c r="E139" s="212" t="s">
         <v>462</v>
       </c>
-      <c r="G139" s="213" t="s">
+      <c r="F139" s="217" t="s">
         <v>463</v>
       </c>
-      <c r="H139" s="227" t="s">
+      <c r="G139" s="217" t="s">
         <v>464</v>
       </c>
-      <c r="I139" s="234" t="s">
+      <c r="H139" s="231" t="s">
         <v>465</v>
       </c>
+      <c r="I139" s="240" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="140" ht="15" spans="1:9">
-      <c r="A140" s="198"/>
-      <c r="B140" s="209" t="s">
-        <v>466</v>
-      </c>
-      <c r="C140" s="207" t="s">
+      <c r="A140" s="202"/>
+      <c r="B140" s="213" t="s">
         <v>467</v>
       </c>
-      <c r="D140" s="208" t="s">
+      <c r="C140" s="211" t="s">
         <v>468</v>
       </c>
-      <c r="E140" s="213" t="s">
+      <c r="D140" s="212" t="s">
         <v>469</v>
       </c>
-      <c r="F140" s="213" t="s">
+      <c r="E140" s="217" t="s">
         <v>470</v>
       </c>
-      <c r="G140" s="213" t="s">
+      <c r="F140" s="217" t="s">
         <v>471</v>
       </c>
-      <c r="H140" s="225" t="s">
+      <c r="G140" s="217" t="s">
         <v>472</v>
       </c>
-      <c r="I140" s="235" t="s">
+      <c r="H140" s="229" t="s">
         <v>473</v>
       </c>
+      <c r="I140" s="241" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="141" ht="15" spans="1:9">
-      <c r="A141" s="198"/>
-      <c r="B141" s="209" t="s">
-        <v>474</v>
-      </c>
-      <c r="C141" s="207" t="s">
+      <c r="A141" s="202"/>
+      <c r="B141" s="213" t="s">
         <v>475</v>
       </c>
-      <c r="D141" s="208" t="s">
+      <c r="C141" s="211" t="s">
         <v>476</v>
       </c>
-      <c r="E141" s="213" t="s">
+      <c r="D141" s="212" t="s">
         <v>477</v>
       </c>
-      <c r="F141" s="213" t="s">
+      <c r="E141" s="217" t="s">
         <v>478</v>
       </c>
-      <c r="G141" s="213" t="s">
+      <c r="F141" s="217" t="s">
         <v>479</v>
       </c>
-      <c r="H141" s="225" t="s">
+      <c r="G141" s="217" t="s">
         <v>480</v>
       </c>
-      <c r="I141" s="235" t="s">
+      <c r="H141" s="229" t="s">
         <v>481</v>
       </c>
+      <c r="I141" s="241" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="142" ht="25.5" spans="1:9">
-      <c r="A142" s="198"/>
-      <c r="B142" s="209" t="s">
-        <v>482</v>
-      </c>
-      <c r="C142" s="207" t="s">
-        <v>444</v>
-      </c>
-      <c r="D142" s="208" t="s">
+      <c r="A142" s="202"/>
+      <c r="B142" s="213" t="s">
         <v>483</v>
       </c>
-      <c r="E142" s="213" t="s">
+      <c r="C142" s="211" t="s">
+        <v>445</v>
+      </c>
+      <c r="D142" s="212" t="s">
         <v>484</v>
       </c>
-      <c r="F142" s="213" t="s">
+      <c r="E142" s="217" t="s">
         <v>485</v>
       </c>
-      <c r="G142" s="213" t="s">
+      <c r="F142" s="217" t="s">
         <v>486</v>
       </c>
-      <c r="H142" s="225" t="s">
+      <c r="G142" s="217" t="s">
         <v>487</v>
       </c>
-      <c r="I142" s="236" t="s">
+      <c r="H142" s="229" t="s">
         <v>488</v>
       </c>
+      <c r="I142" s="242" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="143" ht="15" spans="1:9">
-      <c r="A143" s="198"/>
-      <c r="B143" s="209" t="s">
-        <v>489</v>
-      </c>
-      <c r="C143" s="207" t="s">
+      <c r="A143" s="202"/>
+      <c r="B143" s="213" t="s">
         <v>490</v>
       </c>
-      <c r="D143" s="208" t="s">
+      <c r="C143" s="211" t="s">
         <v>491</v>
       </c>
-      <c r="E143" s="213" t="s">
+      <c r="D143" s="212" t="s">
         <v>492</v>
       </c>
-      <c r="F143" s="213" t="s">
+      <c r="E143" s="217" t="s">
         <v>493</v>
       </c>
-      <c r="G143" s="213" t="s">
+      <c r="F143" s="217" t="s">
         <v>494</v>
       </c>
-      <c r="H143" s="225" t="s">
+      <c r="G143" s="217" t="s">
         <v>495</v>
       </c>
-      <c r="I143" s="235" t="s">
+      <c r="H143" s="229" t="s">
         <v>496</v>
       </c>
+      <c r="I143" s="241" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="144" ht="15" spans="1:9">
-      <c r="A144" s="198"/>
-      <c r="B144" s="209" t="s">
-        <v>497</v>
-      </c>
-      <c r="C144" s="207" t="s">
+      <c r="A144" s="202"/>
+      <c r="B144" s="213" t="s">
         <v>498</v>
       </c>
-      <c r="D144" s="208" t="s">
+      <c r="C144" s="211" t="s">
         <v>499</v>
       </c>
-      <c r="E144" s="213" t="s">
+      <c r="D144" s="212" t="s">
         <v>500</v>
       </c>
-      <c r="F144" s="213" t="s">
+      <c r="E144" s="217" t="s">
         <v>501</v>
       </c>
-      <c r="G144" s="213" t="s">
+      <c r="F144" s="217" t="s">
         <v>502</v>
       </c>
-      <c r="H144" s="225" t="s">
+      <c r="G144" s="217" t="s">
         <v>503</v>
       </c>
-      <c r="I144" s="235" t="s">
+      <c r="H144" s="229" t="s">
         <v>504</v>
       </c>
+      <c r="I144" s="241" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="145" ht="21.75" customHeight="1" spans="1:9">
-      <c r="A145" s="198"/>
-      <c r="B145" s="209" t="s">
-        <v>505</v>
-      </c>
-      <c r="C145" s="207" t="s">
+      <c r="A145" s="202"/>
+      <c r="B145" s="213" t="s">
         <v>506</v>
       </c>
-      <c r="D145" s="208" t="s">
-        <v>475</v>
-      </c>
-      <c r="E145" s="213" t="s">
+      <c r="C145" s="211" t="s">
         <v>507</v>
       </c>
-      <c r="F145" s="213" t="s">
+      <c r="D145" s="212" t="s">
+        <v>476</v>
+      </c>
+      <c r="E145" s="217" t="s">
         <v>508</v>
       </c>
-      <c r="G145" s="213" t="s">
+      <c r="F145" s="217" t="s">
         <v>509</v>
       </c>
-      <c r="H145" s="225" t="s">
+      <c r="G145" s="217" t="s">
         <v>510</v>
       </c>
-      <c r="I145" s="235" t="s">
+      <c r="H145" s="229" t="s">
         <v>511</v>
       </c>
+      <c r="I145" s="241" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="146" ht="25.5" customHeight="1" spans="1:9">
-      <c r="A146" s="198"/>
-      <c r="B146" s="209" t="s">
-        <v>512</v>
-      </c>
-      <c r="C146" s="207" t="s">
-        <v>460</v>
-      </c>
-      <c r="D146" s="208" t="s">
+      <c r="A146" s="202"/>
+      <c r="B146" s="213" t="s">
         <v>513</v>
       </c>
-      <c r="E146" s="213" t="s">
+      <c r="C146" s="211" t="s">
+        <v>461</v>
+      </c>
+      <c r="D146" s="212" t="s">
         <v>514</v>
       </c>
-      <c r="F146" s="213" t="s">
+      <c r="E146" s="217" t="s">
         <v>515</v>
       </c>
-      <c r="G146" s="213" t="s">
+      <c r="F146" s="217" t="s">
         <v>516</v>
       </c>
-      <c r="H146" s="225" t="s">
+      <c r="G146" s="217" t="s">
         <v>517</v>
       </c>
-      <c r="I146" s="237" t="s">
+      <c r="H146" s="229" t="s">
         <v>518</v>
       </c>
+      <c r="I146" s="243" t="s">
+        <v>519</v>
+      </c>
     </row>
     <row r="147" spans="1:9">
-      <c r="A147" s="198"/>
-      <c r="B147" s="209" t="s">
-        <v>519</v>
-      </c>
-      <c r="C147" s="207" t="s">
+      <c r="A147" s="202"/>
+      <c r="B147" s="213" t="s">
         <v>520</v>
       </c>
-      <c r="D147" s="208" t="s">
+      <c r="C147" s="211" t="s">
         <v>521</v>
       </c>
-      <c r="E147" s="213" t="s">
+      <c r="D147" s="212" t="s">
         <v>522</v>
       </c>
-      <c r="F147" s="213" t="s">
+      <c r="E147" s="217" t="s">
         <v>523</v>
       </c>
-      <c r="G147" s="213" t="s">
-        <v>437</v>
-      </c>
-      <c r="H147" s="208" t="s">
+      <c r="F147" s="217" t="s">
         <v>524</v>
       </c>
-      <c r="I147" s="238" t="s">
+      <c r="G147" s="217" t="s">
+        <v>438</v>
+      </c>
+      <c r="H147" s="212" t="s">
         <v>525</v>
       </c>
+      <c r="I147" s="233" t="s">
+        <v>526</v>
+      </c>
     </row>
     <row r="148" spans="1:9">
-      <c r="A148" s="198"/>
-      <c r="B148" s="210" t="s">
+      <c r="A148" s="202"/>
+      <c r="B148" s="214" t="s">
+        <v>527</v>
+      </c>
+      <c r="C148" s="211" t="s">
+        <v>528</v>
+      </c>
+      <c r="D148" s="212" t="s">
+        <v>529</v>
+      </c>
+      <c r="E148" s="217" t="s">
+        <v>530</v>
+      </c>
+      <c r="F148" s="217" t="s">
+        <v>531</v>
+      </c>
+      <c r="G148" s="217" t="s">
+        <v>532</v>
+      </c>
+      <c r="H148" s="212" t="s">
+        <v>533</v>
+      </c>
+      <c r="I148" s="233" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9">
+      <c r="A149" s="202"/>
+      <c r="B149" s="214" t="s">
+        <v>478</v>
+      </c>
+      <c r="C149" s="211" t="s">
+        <v>535</v>
+      </c>
+      <c r="D149" s="212" t="s">
+        <v>536</v>
+      </c>
+      <c r="E149" s="217" t="s">
+        <v>537</v>
+      </c>
+      <c r="F149" s="217" t="s">
+        <v>538</v>
+      </c>
+      <c r="G149" s="217" t="s">
+        <v>539</v>
+      </c>
+      <c r="H149" s="212" t="s">
+        <v>540</v>
+      </c>
+      <c r="I149" s="233" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9">
+      <c r="A150" s="202"/>
+      <c r="B150" s="214" t="s">
+        <v>542</v>
+      </c>
+      <c r="C150" s="211" t="s">
+        <v>543</v>
+      </c>
+      <c r="D150" s="212" t="s">
+        <v>544</v>
+      </c>
+      <c r="E150" s="217" t="s">
+        <v>545</v>
+      </c>
+      <c r="F150" s="217" t="s">
+        <v>546</v>
+      </c>
+      <c r="G150" s="217" t="s">
+        <v>547</v>
+      </c>
+      <c r="H150" s="212" t="s">
+        <v>548</v>
+      </c>
+      <c r="I150" s="233" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="151" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A151" s="202"/>
+      <c r="B151" s="214" t="s">
+        <v>550</v>
+      </c>
+      <c r="C151" s="215" t="s">
+        <v>551</v>
+      </c>
+      <c r="D151" s="216" t="s">
+        <v>552</v>
+      </c>
+      <c r="E151" s="217" t="s">
+        <v>553</v>
+      </c>
+      <c r="F151" s="217" t="s">
+        <v>554</v>
+      </c>
+      <c r="G151" s="217" t="s">
+        <v>555</v>
+      </c>
+      <c r="H151" s="212" t="s">
+        <v>556</v>
+      </c>
+      <c r="I151" s="233" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9">
+      <c r="A152" s="202"/>
+      <c r="B152" s="214" t="s">
+        <v>558</v>
+      </c>
+      <c r="C152" s="217" t="s">
+        <v>559</v>
+      </c>
+      <c r="D152" s="217" t="s">
+        <v>560</v>
+      </c>
+      <c r="E152" s="217" t="s">
+        <v>561</v>
+      </c>
+      <c r="F152" s="217" t="s">
+        <v>524</v>
+      </c>
+      <c r="G152" s="217" t="s">
+        <v>562</v>
+      </c>
+      <c r="H152" s="212" t="s">
+        <v>563</v>
+      </c>
+      <c r="I152" s="233" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="153" ht="28.5" spans="1:9">
+      <c r="A153" s="202"/>
+      <c r="B153" s="218" t="s">
+        <v>565</v>
+      </c>
+      <c r="C153" s="219" t="s">
+        <v>566</v>
+      </c>
+      <c r="D153" s="212" t="s">
+        <v>567</v>
+      </c>
+      <c r="E153" s="212" t="s">
+        <v>568</v>
+      </c>
+      <c r="F153" s="230" t="s">
+        <v>569</v>
+      </c>
+      <c r="G153" s="230" t="s">
+        <v>570</v>
+      </c>
+      <c r="H153" s="232" t="s">
+        <v>571</v>
+      </c>
+      <c r="I153" s="234" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="154" ht="15" spans="1:9">
+      <c r="A154" s="220"/>
+      <c r="B154" s="221" t="s">
+        <v>573</v>
+      </c>
+      <c r="C154" s="222"/>
+      <c r="D154" s="222"/>
+      <c r="E154" s="222"/>
+      <c r="F154" s="233" t="s">
         <v>526</v>
       </c>
-      <c r="C148" s="207" t="s">
-        <v>527</v>
-      </c>
-      <c r="D148" s="208" t="s">
-        <v>528</v>
-      </c>
-      <c r="E148" s="213" t="s">
-        <v>529</v>
-      </c>
-      <c r="F148" s="213" t="s">
-        <v>530</v>
-      </c>
-      <c r="G148" s="213" t="s">
-        <v>531</v>
-      </c>
-      <c r="H148" s="208" t="s">
-        <v>532</v>
-      </c>
-      <c r="I148" s="238" t="s">
+      <c r="G154" s="222" t="s">
+        <v>525</v>
+      </c>
+      <c r="H154" s="230" t="s">
+        <v>574</v>
+      </c>
+      <c r="I154" s="234" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="155" ht="15" spans="6:8">
+      <c r="F155" s="233" t="s">
+        <v>534</v>
+      </c>
+      <c r="G155" s="2" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="149" spans="1:9">
-      <c r="A149" s="198"/>
-      <c r="B149" s="210" t="s">
-        <v>477</v>
-      </c>
-      <c r="C149" s="207" t="s">
-        <v>534</v>
-      </c>
-      <c r="D149" s="208" t="s">
-        <v>535</v>
-      </c>
-      <c r="E149" s="213" t="s">
-        <v>536</v>
-      </c>
-      <c r="F149" s="213" t="s">
-        <v>537</v>
-      </c>
-      <c r="G149" s="213" t="s">
-        <v>538</v>
-      </c>
-      <c r="H149" s="208" t="s">
-        <v>539</v>
-      </c>
-      <c r="I149" s="238" t="s">
+      <c r="H155" s="222"/>
+    </row>
+    <row r="156" spans="6:7">
+      <c r="F156" s="233" t="s">
+        <v>541</v>
+      </c>
+      <c r="G156" s="2" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="150" spans="1:9">
-      <c r="A150" s="198"/>
-      <c r="B150" s="210" t="s">
-        <v>541</v>
-      </c>
-      <c r="C150" s="207" t="s">
-        <v>542</v>
-      </c>
-      <c r="D150" s="208" t="s">
-        <v>543</v>
-      </c>
-      <c r="E150" s="213" t="s">
-        <v>544</v>
-      </c>
-      <c r="F150" s="213" t="s">
-        <v>545</v>
-      </c>
-      <c r="G150" s="213" t="s">
-        <v>546</v>
-      </c>
-      <c r="H150" s="208" t="s">
-        <v>547</v>
-      </c>
-      <c r="I150" s="238" t="s">
+    <row r="157" spans="6:7">
+      <c r="F157" s="233" t="s">
+        <v>549</v>
+      </c>
+      <c r="G157" s="2" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="151" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A151" s="198"/>
-      <c r="B151" s="210" t="s">
-        <v>549</v>
-      </c>
-      <c r="C151" s="211" t="s">
-        <v>550</v>
-      </c>
-      <c r="D151" s="212" t="s">
-        <v>551</v>
-      </c>
-      <c r="E151" s="213" t="s">
-        <v>552</v>
-      </c>
-      <c r="F151" s="213" t="s">
-        <v>553</v>
-      </c>
-      <c r="G151" s="213" t="s">
-        <v>554</v>
-      </c>
-      <c r="H151" s="208" t="s">
-        <v>555</v>
-      </c>
-      <c r="I151" s="238" t="s">
+    <row r="158" ht="28.5" spans="6:7">
+      <c r="F158" s="233" t="s">
+        <v>557</v>
+      </c>
+      <c r="G158" s="2" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="152" spans="1:9">
-      <c r="A152" s="198"/>
-      <c r="B152" s="210" t="s">
-        <v>557</v>
-      </c>
-      <c r="C152" s="213" t="s">
-        <v>558</v>
-      </c>
-      <c r="D152" s="213" t="s">
-        <v>559</v>
-      </c>
-      <c r="E152" s="213" t="s">
-        <v>560</v>
-      </c>
-      <c r="F152" s="213" t="s">
-        <v>523</v>
-      </c>
-      <c r="G152" s="213" t="s">
-        <v>561</v>
-      </c>
-      <c r="H152" s="208" t="s">
-        <v>562</v>
-      </c>
-      <c r="I152" s="238" t="s">
+    <row r="159" spans="6:7">
+      <c r="F159" s="233" t="s">
+        <v>564</v>
+      </c>
+      <c r="G159" s="2" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="153" ht="28.5" spans="1:9">
-      <c r="A153" s="198"/>
-      <c r="B153" s="214" t="s">
-        <v>564</v>
-      </c>
-      <c r="C153" s="215" t="s">
-        <v>565</v>
-      </c>
-      <c r="D153" s="208" t="s">
-        <v>566</v>
-      </c>
-      <c r="E153" s="208" t="s">
-        <v>567</v>
-      </c>
-      <c r="F153" s="226" t="s">
-        <v>568</v>
-      </c>
-      <c r="G153" s="226" t="s">
-        <v>569</v>
-      </c>
-      <c r="H153" s="228" t="s">
-        <v>570</v>
-      </c>
-      <c r="I153" s="239" t="s">
+    <row r="160" spans="6:7">
+      <c r="F160" s="234" t="s">
+        <v>572</v>
+      </c>
+      <c r="G160" s="2" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="154" ht="15" spans="1:9">
-      <c r="A154" s="216"/>
-      <c r="B154" s="217" t="s">
-        <v>572</v>
-      </c>
-      <c r="C154" s="218"/>
-      <c r="D154" s="218"/>
-      <c r="E154" s="218"/>
-      <c r="F154" s="218"/>
-      <c r="G154" s="218"/>
-      <c r="H154" s="226" t="s">
-        <v>573</v>
-      </c>
-      <c r="I154" s="239" t="s">
+    <row r="161" ht="28.5" spans="6:7">
+      <c r="F161" s="234" t="s">
+        <v>575</v>
+      </c>
+      <c r="G161" s="2" t="s">
         <v>574</v>
       </c>
-    </row>
-    <row r="155" spans="8:8">
-      <c r="H155" s="218"/>
     </row>
     <row r="191" spans="5:5">
       <c r="E191"/>
     </row>
   </sheetData>
-  <mergeCells count="135">
+  <mergeCells count="137">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="B13:C13"/>
@@ -7284,8 +7355,10 @@
     <mergeCell ref="F76:G76"/>
     <mergeCell ref="B77:C77"/>
     <mergeCell ref="F77:G77"/>
+    <mergeCell ref="H77:I77"/>
     <mergeCell ref="B78:C78"/>
     <mergeCell ref="F78:G78"/>
+    <mergeCell ref="H78:I78"/>
     <mergeCell ref="B79:C79"/>
     <mergeCell ref="B80:C80"/>
     <mergeCell ref="B81:D81"/>
@@ -7363,32 +7436,32 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>